<commit_message>
SummentitelXX sind nun PublicVariablen und werden ebenfalls mit Engl./Deutschen Texten besetzt;  .copy()/.paste() wurden für alle Shapes für die Reports durch pptCopypptPaste-Aufruf oder xlnsCopypptPaste-Aufruf ersetzt. Hierin werden mehrer Versuche gemacht den copy/paste auszuführen, um zu verhindern, dass die Meldung 'unkown Shapes' auftaucht. kleine Korrekturen an den englischen Texte; summentitel-Texte hinzugefügt
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\Documents\Visual Studio 2013\Projects\ProjectBoard\Projectboard\ClassLibrary1\My Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\Documents\Visual Studio 2013\Projects\ProjectBoard\Projectboard\ClassLibrary1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="499">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -791,9 +791,6 @@
     <t xml:space="preserve">no achieved targets </t>
   </si>
   <si>
-    <t>Phase</t>
-  </si>
-  <si>
     <t xml:space="preserve">not defined: </t>
   </si>
   <si>
@@ -1049,9 +1046,6 @@
     <t>Fortschritt Gesamtkosten</t>
   </si>
   <si>
-    <t>kennzeichnung</t>
-  </si>
-  <si>
     <t>Fortschritt Rolle</t>
   </si>
   <si>
@@ -1187,18 +1181,9 @@
     <t>Overview Better/Worse</t>
   </si>
   <si>
-    <t>Overview Utilization</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (FTE)</t>
   </si>
   <si>
-    <t>Details below-Capacity</t>
-  </si>
-  <si>
-    <t>Details above-Capacity</t>
-  </si>
-  <si>
     <t>Current Target Achievements</t>
   </si>
   <si>
@@ -1214,9 +1199,6 @@
     <t>Traffic Light Explanation</t>
   </si>
   <si>
-    <t>Business Unit</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -1473,6 +1455,72 @@
   </si>
   <si>
     <t xml:space="preserve">all projects with costs  </t>
+  </si>
+  <si>
+    <t>Prognose Ergebniskennzahl</t>
+  </si>
+  <si>
+    <t>strategischer Fit, Risiko &amp; Marge</t>
+  </si>
+  <si>
+    <t>Personal-Kosten intern/extern</t>
+  </si>
+  <si>
+    <t>Personal Kosten Struktur</t>
+  </si>
+  <si>
+    <t>Ergebnis Verbesserungs-Potentiale</t>
+  </si>
+  <si>
+    <t>Bisherige Ziel-Erreichung</t>
+  </si>
+  <si>
+    <t>Prognose zukünftige Ziel-Erreichung</t>
+  </si>
+  <si>
+    <t>Bisherige &amp; zukünftige Ziel-Erreichung</t>
+  </si>
+  <si>
+    <t>Auslastungs-Übersicht</t>
+  </si>
+  <si>
+    <t>Details zur Über-Auslastung</t>
+  </si>
+  <si>
+    <t>Details zur Unter-Auslastung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase </t>
+  </si>
+  <si>
+    <t>Forecast Result</t>
+  </si>
+  <si>
+    <t>strategic Fit, Risk &amp; Margin</t>
+  </si>
+  <si>
+    <t>Personnel Cost intern/extern</t>
+  </si>
+  <si>
+    <t>Personnel Cost Structure</t>
+  </si>
+  <si>
+    <t>Overview Capacity Utilization</t>
+  </si>
+  <si>
+    <t>Details Capacity Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Free Capacity </t>
+  </si>
+  <si>
+    <t>Current &amp; Forecast Target Achievements</t>
+  </si>
+  <si>
+    <t>Business Unit:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Unit </t>
   </si>
 </sst>
 </file>
@@ -1807,10 +1855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:C248"/>
+  <dimension ref="A1:B259"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="B118" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="B209" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1944,7 +1992,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,7 +2000,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1960,7 +2008,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,7 +2016,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +2040,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +2048,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2120,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,7 +2144,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2168,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2192,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2200,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2208,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2216,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2224,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2232,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2240,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2248,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2216,7 +2264,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2272,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,7 +2280,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2240,15 +2288,15 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2304,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,7 +2312,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2320,7 @@
         <v>50</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,7 +2328,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2288,7 +2336,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,7 +2344,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2304,7 +2352,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2312,7 +2360,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2320,7 +2368,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2328,7 +2376,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2336,7 +2384,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2384,7 +2432,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2392,7 +2440,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2448,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,7 +2456,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2416,7 +2464,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,7 +2472,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,7 +2480,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2448,7 +2496,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2504,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2544,7 +2592,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,7 +2600,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2568,7 +2616,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2576,7 +2624,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2592,7 +2640,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +2680,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2688,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2696,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2664,7 +2712,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,7 +2744,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>255</v>
+        <v>488</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2704,7 +2752,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,7 +2760,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2720,7 +2768,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2728,7 +2776,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2736,7 +2784,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,7 +2792,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2752,7 +2800,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2760,7 +2808,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2768,7 +2816,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,7 +2832,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2792,7 +2840,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2800,7 +2848,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2808,7 +2856,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2816,7 +2864,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2824,7 +2872,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2832,7 +2880,7 @@
         <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2840,7 +2888,7 @@
         <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,7 +2896,7 @@
         <v>126</v>
       </c>
       <c r="B129" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2856,7 +2904,7 @@
         <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2864,7 +2912,7 @@
         <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2872,7 +2920,7 @@
         <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2880,7 +2928,7 @@
         <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2888,7 +2936,7 @@
         <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2896,7 +2944,7 @@
         <v>132</v>
       </c>
       <c r="B135" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2904,7 +2952,7 @@
         <v>133</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2912,7 +2960,7 @@
         <v>134</v>
       </c>
       <c r="B137" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2920,7 +2968,7 @@
         <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2928,7 +2976,7 @@
         <v>120</v>
       </c>
       <c r="B139" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2936,7 +2984,7 @@
         <v>136</v>
       </c>
       <c r="B140" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,7 +2992,7 @@
         <v>137</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,7 +3000,7 @@
         <v>138</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2960,7 +3008,7 @@
         <v>139</v>
       </c>
       <c r="B143" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2968,7 +3016,7 @@
         <v>140</v>
       </c>
       <c r="B144" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +3024,7 @@
         <v>141</v>
       </c>
       <c r="B145" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +3032,7 @@
         <v>142</v>
       </c>
       <c r="B146" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +3048,7 @@
         <v>144</v>
       </c>
       <c r="B148" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3056,7 @@
         <v>145</v>
       </c>
       <c r="B149" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3064,7 @@
         <v>146</v>
       </c>
       <c r="B150" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3072,7 @@
         <v>147</v>
       </c>
       <c r="B151" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3080,7 @@
         <v>137</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3088,7 @@
         <v>148</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3096,7 @@
         <v>149</v>
       </c>
       <c r="B154" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3104,7 @@
         <v>150</v>
       </c>
       <c r="B155" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3112,7 @@
         <v>151</v>
       </c>
       <c r="B156" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3120,7 @@
         <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3128,7 @@
         <v>153</v>
       </c>
       <c r="B158" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3136,7 @@
         <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3144,7 @@
         <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3160,7 @@
         <v>157</v>
       </c>
       <c r="B162" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3168,7 @@
         <v>158</v>
       </c>
       <c r="B163" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3128,7 +3176,7 @@
         <v>51</v>
       </c>
       <c r="B164" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3184,7 @@
         <v>159</v>
       </c>
       <c r="B165" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3192,7 @@
         <v>160</v>
       </c>
       <c r="B166" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3200,7 @@
         <v>161</v>
       </c>
       <c r="B167" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3208,7 @@
         <v>162</v>
       </c>
       <c r="B168" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3216,7 @@
         <v>163</v>
       </c>
       <c r="B169" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3224,7 @@
         <v>164</v>
       </c>
       <c r="B170" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3232,7 @@
         <v>165</v>
       </c>
       <c r="B171" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3192,7 +3240,7 @@
         <v>166</v>
       </c>
       <c r="B172" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,7 +3256,7 @@
         <v>167</v>
       </c>
       <c r="B174" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -3216,7 +3264,7 @@
         <v>168</v>
       </c>
       <c r="B175" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -3224,7 +3272,7 @@
         <v>169</v>
       </c>
       <c r="B176" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3232,7 +3280,7 @@
         <v>170</v>
       </c>
       <c r="B177" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,7 +3288,7 @@
         <v>171</v>
       </c>
       <c r="B178" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3248,7 +3296,7 @@
         <v>172</v>
       </c>
       <c r="B179" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3256,7 +3304,7 @@
         <v>173</v>
       </c>
       <c r="B180" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3264,7 +3312,7 @@
         <v>174</v>
       </c>
       <c r="B181" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3272,7 +3320,7 @@
         <v>175</v>
       </c>
       <c r="B182" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3280,7 +3328,7 @@
         <v>176</v>
       </c>
       <c r="B183" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3336,7 @@
         <v>26</v>
       </c>
       <c r="B184" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3344,7 @@
         <v>177</v>
       </c>
       <c r="B185" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3352,7 @@
         <v>178</v>
       </c>
       <c r="B186" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3312,7 +3360,7 @@
         <v>179</v>
       </c>
       <c r="B187" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,7 +3368,7 @@
         <v>180</v>
       </c>
       <c r="B188" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3328,7 +3376,7 @@
         <v>181</v>
       </c>
       <c r="B189" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3336,7 +3384,7 @@
         <v>182</v>
       </c>
       <c r="B190" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3344,7 +3392,7 @@
         <v>183</v>
       </c>
       <c r="B191" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3352,458 +3400,543 @@
         <v>184</v>
       </c>
       <c r="B192" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>185</v>
       </c>
       <c r="B193" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>186</v>
       </c>
       <c r="B194" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>187</v>
       </c>
       <c r="B195" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>188</v>
       </c>
       <c r="B196" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>189</v>
       </c>
       <c r="B197" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>190</v>
       </c>
       <c r="B198" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>191</v>
       </c>
       <c r="B199" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>192</v>
       </c>
       <c r="B200" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>193</v>
       </c>
       <c r="B201" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>194</v>
       </c>
       <c r="B202" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>195</v>
       </c>
       <c r="B203" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>337</v>
+      </c>
+      <c r="B205" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>338</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>339</v>
+      </c>
+      <c r="B207" t="s">
         <v>375</v>
       </c>
-      <c r="C205" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>339</v>
-      </c>
-      <c r="B206" t="s">
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>340</v>
+      </c>
+      <c r="B208" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>340</v>
-      </c>
-      <c r="B207" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>342</v>
-      </c>
-      <c r="B208" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B209" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B210" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B211" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B212" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B213" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B214" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B215" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B216" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B217" t="s">
-        <v>387</v>
+        <v>493</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B218" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B219" t="s">
-        <v>389</v>
+        <v>494</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B220" t="s">
-        <v>390</v>
+        <v>495</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B221" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B222" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B223" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B224" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B225" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B226" t="s">
-        <v>396</v>
+        <v>497</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B227" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B228" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B229" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B230" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B231" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B232" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B233" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B234" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B235" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B236" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B237" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B238" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B239" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B240" t="s">
-        <v>396</v>
+        <v>498</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B241" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B242" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="B243" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B244" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B245" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B246" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B247" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B248" t="s">
-        <v>470</v>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>477</v>
+      </c>
+      <c r="B249" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>478</v>
+      </c>
+      <c r="B250" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>479</v>
+      </c>
+      <c r="B251" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>480</v>
+      </c>
+      <c r="B252" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>481</v>
+      </c>
+      <c r="B253" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>482</v>
+      </c>
+      <c r="B254" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>483</v>
+      </c>
+      <c r="B255" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>484</v>
+      </c>
+      <c r="B256" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>485</v>
+      </c>
+      <c r="B257" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>486</v>
+      </c>
+      <c r="B258" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>487</v>
+      </c>
+      <c r="B259" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Korrktur: repMessages.getmsg(260) = Interne Kapazität; diese Message fehlte ganz. teilweise vor oder hinter die engl. Message Leerzeichen eingefügt.
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="505">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -32,21 +32,12 @@
     <t>Shape für Legenden-Liste hat keine Tabelle</t>
   </si>
   <si>
-    <t>Tabelle hat keine durch 3 teilbare Anzahl Spalten &amp; vbLf &amp; Symbol, Short- und Long-Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tabelle muss mindestens 2 Zeilen haben .... </t>
   </si>
   <si>
     <t>Produktlinie ist undefiniert</t>
   </si>
   <si>
-    <t xml:space="preserve">Anzahl Zeilen in der Tabelle sind nicht ausreichend. &amp; vbLf &amp; Tabelle muss anders definiert werden .... </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die LegendenTabelle wird zu groß für eine Seite. &amp; vbLf &amp; Tabelle muss anders definiert werden .... </t>
-  </si>
-  <si>
     <t xml:space="preserve">die Legenden Symbole Phase oder Meilenstein fehlen </t>
   </si>
   <si>
@@ -71,9 +62,6 @@
     <t xml:space="preserve"> ohne Name</t>
   </si>
   <si>
-    <t xml:space="preserve"> Projekt, ggf. mit &amp; vbLf &amp; Anfangs- und Ende-Markierung</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Platz für die Legende reicht nicht aus. Evt.muss eine neue Vorlage definiert werden!</t>
   </si>
   <si>
@@ -92,9 +80,6 @@
     <t xml:space="preserve">Meilenstein Trendanalyse </t>
   </si>
   <si>
-    <t xml:space="preserve"> zum diesem Projekt gibt es noch keine Trend-Analyse, &amp; vbLf &amp; da es noch nicht begonnen hat</t>
-  </si>
-  <si>
     <t xml:space="preserve">  es gibt keine Meilensteine im Projekt</t>
   </si>
   <si>
@@ -134,9 +119,6 @@
     <t xml:space="preserve"> Ende: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Tabelle Projektänderungen hat evtl unzulässige Anzahl Zeilen / Spalten ...</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Anzahl der Zeilen oder Spalten in der Projektstatus Tabelle passt nicht ...</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
     <t xml:space="preserve"> letzter Stand </t>
   </si>
   <si>
-    <t xml:space="preserve">  Tage</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Monate</t>
   </si>
   <si>
@@ -182,12 +161,6 @@
     <t xml:space="preserve"> Personalkosten</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sonstige Kosten</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ergebnis-Prognose</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Earned Value - gewichtet</t>
   </si>
   <si>
@@ -263,24 +236,15 @@
     <t xml:space="preserve"> Prozentuale  </t>
   </si>
   <si>
-    <t>Datenbank-Verbindung ist unterbrochen! &amp; vbLf &amp; Projekthistorie konnte nicht geladen werden</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Fehler in CreateBetterWorsePortfolio  </t>
   </si>
   <si>
     <t xml:space="preserve"> es gibt keine Projekte mit Abweichungen, die größer als die tolerierten Werte sind </t>
   </si>
   <si>
-    <t xml:space="preserve"> Zeit-Toleranz Projekt-Ende: +/- </t>
-  </si>
-  <si>
     <t xml:space="preserve">  Zeit-Toleranz nächster Meilenstein: +/-</t>
   </si>
   <si>
-    <t xml:space="preserve"> Zeit-Toleranz: +/- </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Kosten-Toleranz: +/-</t>
   </si>
   <si>
@@ -374,9 +338,6 @@
     <t xml:space="preserve"> Risiko Abschlag</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kapazität incl. Externe</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Leistbarkeitsgrenze</t>
   </si>
   <si>
@@ -530,9 +491,6 @@
     <t xml:space="preserve"> Risikokosten</t>
   </si>
   <si>
-    <t xml:space="preserve">  progn.Ergebnis</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Fortschritt </t>
   </si>
   <si>
@@ -647,9 +605,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>please use another template - projects do not fit to one page ???</t>
-  </si>
-  <si>
     <t>without name</t>
   </si>
   <si>
@@ -662,9 +617,6 @@
     <t>Milestone Trendanalysis</t>
   </si>
   <si>
-    <t>project template does not exist</t>
-  </si>
-  <si>
     <t xml:space="preserve">template could not be found </t>
   </si>
   <si>
@@ -695,15 +647,9 @@
     <t>identical</t>
   </si>
   <si>
-    <t>table project changes with wrong number of rows / columns</t>
-  </si>
-  <si>
     <t xml:space="preserve">number of rows and columns does not fit to project status table </t>
   </si>
   <si>
-    <t>there is no trend for that project</t>
-  </si>
-  <si>
     <t>no milestones specified</t>
   </si>
   <si>
@@ -761,9 +707,6 @@
     <t>Cost deviation</t>
   </si>
   <si>
-    <t>Capacity utilization</t>
-  </si>
-  <si>
     <t>no resource needs defined</t>
   </si>
   <si>
@@ -782,15 +725,6 @@
     <t xml:space="preserve">no forecast: time frame entirely in past </t>
   </si>
   <si>
-    <t>no future targets defined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no achieved nor future targets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">no achieved targets </t>
-  </si>
-  <si>
     <t xml:space="preserve">not defined: </t>
   </si>
   <si>
@@ -812,18 +746,12 @@
     <t xml:space="preserve">Capacity incl. Ext. </t>
   </si>
   <si>
-    <t>Milestone</t>
-  </si>
-  <si>
     <t>not existent</t>
   </si>
   <si>
     <t xml:space="preserve">no table for scenario </t>
   </si>
   <si>
-    <t>no time frame provided in table</t>
-  </si>
-  <si>
     <t>no elements provided ….</t>
   </si>
   <si>
@@ -836,9 +764,6 @@
     <t>no projects in given time frame</t>
   </si>
   <si>
-    <t>please provide time frame …</t>
-  </si>
-  <si>
     <t>no phases provided …</t>
   </si>
   <si>
@@ -881,9 +806,6 @@
     <t>less expensive</t>
   </si>
   <si>
-    <t>history strategic fit &amp; risk</t>
-  </si>
-  <si>
     <t xml:space="preserve">no project history yet </t>
   </si>
   <si>
@@ -923,9 +845,6 @@
     <t>Load</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t xml:space="preserve"> not possible …</t>
   </si>
   <si>
@@ -956,9 +875,6 @@
     <t xml:space="preserve"> no milestones in project</t>
   </si>
   <si>
-    <t xml:space="preserve"> does not exist</t>
-  </si>
-  <si>
     <t xml:space="preserve"> End: </t>
   </si>
   <si>
@@ -974,9 +890,6 @@
     <t xml:space="preserve"> (latest version)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Risk fee</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Overview Phases</t>
   </si>
   <si>
@@ -1019,15 +932,6 @@
     <t xml:space="preserve"> Risk</t>
   </si>
   <si>
-    <t xml:space="preserve"> absolut</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> proportional</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> internal</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;not named&gt;</t>
   </si>
   <si>
@@ -1073,18 +977,9 @@
     <t>Übersicht Besser/Schlechter</t>
   </si>
   <si>
-    <t>Übersicht Auslastung</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (PT)</t>
   </si>
   <si>
-    <t>Details Unterauslastung</t>
-  </si>
-  <si>
-    <t>Details Überauslastung</t>
-  </si>
-  <si>
     <t>Bisherige Zielerreichung</t>
   </si>
   <si>
@@ -1244,27 +1139,9 @@
     <t>Reporting Periods</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Approved Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> latest version</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Personnel Costs</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (approved version)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Other Costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Result Forecast</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Earned Value - rated </t>
   </si>
   <si>
@@ -1274,12 +1151,6 @@
     <t xml:space="preserve"> Risk Fee</t>
   </si>
   <si>
-    <t>Projects within tolerance (+/-</t>
-  </si>
-  <si>
-    <t>Projects without latest version</t>
-  </si>
-  <si>
     <t>above Capacity</t>
   </si>
   <si>
@@ -1307,9 +1178,6 @@
     <t>Cost Forecast</t>
   </si>
   <si>
-    <t>Personnel Needs</t>
-  </si>
-  <si>
     <t>Personnel Costs (T€)</t>
   </si>
   <si>
@@ -1325,9 +1193,6 @@
     <t>Other Costs</t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">sum Other Cost is zero </t>
   </si>
   <si>
@@ -1337,9 +1202,6 @@
     <t>strategic Fit</t>
   </si>
   <si>
-    <t>History of KPI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cost of Risk </t>
   </si>
   <si>
@@ -1379,12 +1241,6 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>target-/actual Role Needs</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">target-/actual Cost </t>
   </si>
   <si>
@@ -1521,6 +1377,168 @@
   </si>
   <si>
     <t xml:space="preserve">Business Unit </t>
+  </si>
+  <si>
+    <t>Tabelle hat keine durch 3 teilbare Anzahl Spalten &amp; vblf &amp; Symbol, Short- und Long-Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl Zeilen in der Tabelle sind nicht ausreichend. &amp; vblf &amp; Tabelle muss anders definiert werden .... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die LegendenTabelle wird zu groß für eine Seite. &amp; vblf &amp; Tabelle muss anders definiert werden .... </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projekt, ggf. mit &amp; vblf &amp; Anfangs- und Ende-Markierung</t>
+  </si>
+  <si>
+    <t>Datenbank-Verbindung ist unterbrochen! &amp; vblf &amp; Projekthistorie konnte nicht geladen werden</t>
+  </si>
+  <si>
+    <t>Interne Kapazität</t>
+  </si>
+  <si>
+    <t>Internal Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">please use another template - projects do not fit to one page ???  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zu diesem Projekt gibt es noch keine Trend-Analyse, &amp; vblf &amp; da es noch nicht begonnen hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project template does not exist  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  does not exist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabelle Projektänderungen hat evtl unzulässige Anzahl Zeilen / Spalten …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table project changes with wrong number of rows / columns </t>
+  </si>
+  <si>
+    <t>there is no trend for that project '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approved Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> latest version </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tage</t>
+  </si>
+  <si>
+    <t>Risiko-Abschlag</t>
+  </si>
+  <si>
+    <t>Personalkosten</t>
+  </si>
+  <si>
+    <t>Ergebnis-Prognose</t>
+  </si>
+  <si>
+    <t>Risk fee</t>
+  </si>
+  <si>
+    <t>Personnel Costs</t>
+  </si>
+  <si>
+    <t>Result Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> absolut </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> proportional  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zeit-Toleranz Projekt-Ende: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zeit-Toleranz: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projects within tolerance (+/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projects without latest version</t>
+  </si>
+  <si>
+    <t>no achieved targets …</t>
+  </si>
+  <si>
+    <t>no future targets defined …</t>
+  </si>
+  <si>
+    <t>no achieved nor future targets …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> internal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity utilization </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kapazität inkl. Externe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> not existent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no time frame provided in table </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> please provide time frame …</t>
+  </si>
+  <si>
+    <t>additional costs due to above-capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personnel Needs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">history strategic fit &amp; risk: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">History of KPI </t>
+  </si>
+  <si>
+    <t>progn. Ergebnis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role </t>
+  </si>
+  <si>
+    <t xml:space="preserve">target-/actual Role Needs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Übersicht Auslastung </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview Capacity Utilization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Unterauslastung </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Capacity Overload </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details Überauslastung </t>
   </si>
 </sst>
 </file>
@@ -1855,10 +1873,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B259"/>
+  <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="B209" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A236" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A249" sqref="A249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,1623 +1890,1623 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>451</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>453</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>454</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>459</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>460</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>461</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>462</v>
       </c>
       <c r="B36" t="s">
-        <v>223</v>
+        <v>463</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>404</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>225</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>405</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>406</v>
+        <v>465</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>407</v>
+        <v>466</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>408</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>468</v>
       </c>
       <c r="B45" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>410</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>469</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>316</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>470</v>
       </c>
       <c r="B51" t="s">
-        <v>409</v>
+        <v>473</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>471</v>
       </c>
       <c r="B53" t="s">
-        <v>412</v>
+        <v>474</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="B54" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>414</v>
+        <v>373</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>415</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>318</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>322</v>
+        <v>293</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B74" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>329</v>
+        <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B79" t="s">
-        <v>331</v>
+        <v>475</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>332</v>
+        <v>476</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>455</v>
       </c>
       <c r="B81" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>477</v>
       </c>
       <c r="B84" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>478</v>
       </c>
       <c r="B86" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B87" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>416</v>
+        <v>479</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>417</v>
+        <v>480</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B93" t="s">
-        <v>245</v>
+        <v>485</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B96" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B97" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B98" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B100" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B101" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>420</v>
+        <v>377</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>421</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B105" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B106" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>254</v>
+        <v>481</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>252</v>
+        <v>482</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B109" t="s">
-        <v>253</v>
+        <v>483</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B110" t="s">
-        <v>488</v>
+        <v>440</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B112" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B114" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B115" t="s">
-        <v>333</v>
+        <v>484</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B117" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>486</v>
       </c>
       <c r="B118" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B121" t="s">
-        <v>262</v>
+        <v>487</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B122" t="s">
-        <v>263</v>
+        <v>488</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B123" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B124" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>265</v>
+        <v>489</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B128" t="s">
-        <v>470</v>
+        <v>422</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B129" t="s">
-        <v>471</v>
+        <v>423</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B130" t="s">
-        <v>472</v>
+        <v>424</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B131" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B132" t="s">
-        <v>473</v>
+        <v>425</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B133" t="s">
-        <v>474</v>
+        <v>426</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B134" t="s">
-        <v>475</v>
+        <v>427</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B135" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B136" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B137" t="s">
-        <v>270</v>
+        <v>490</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B138" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B139" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B140" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>274</v>
+        <v>491</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B143" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B144" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B145" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B146" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B147" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B148" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B149" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B150" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B151" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B154" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B155" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B157" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B158" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B159" t="s">
-        <v>427</v>
+        <v>492</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B160" t="s">
-        <v>428</v>
+        <v>384</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B161" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B162" t="s">
-        <v>429</v>
+        <v>385</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>430</v>
+        <v>386</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>431</v>
+        <v>387</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B165" t="s">
-        <v>432</v>
+        <v>388</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B166" t="s">
-        <v>433</v>
+        <v>493</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B167" t="s">
-        <v>434</v>
+        <v>389</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B168" t="s">
-        <v>435</v>
+        <v>390</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B169" t="s">
-        <v>285</v>
+        <v>494</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B170" t="s">
-        <v>436</v>
+        <v>391</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B171" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B172" t="s">
-        <v>437</v>
+        <v>495</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B173" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B174" t="s">
-        <v>438</v>
+        <v>392</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>168</v>
+        <v>496</v>
       </c>
       <c r="B175" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B176" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B177" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B178" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B179" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B180" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B181" t="s">
-        <v>439</v>
+        <v>393</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B182" t="s">
-        <v>440</v>
+        <v>394</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B183" t="s">
-        <v>441</v>
+        <v>395</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>442</v>
+        <v>396</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B185" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B186" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B187" t="s">
-        <v>443</v>
+        <v>397</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B188" t="s">
-        <v>444</v>
+        <v>398</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B189" t="s">
-        <v>445</v>
+        <v>399</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B190" t="s">
-        <v>446</v>
+        <v>400</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B191" t="s">
-        <v>447</v>
+        <v>401</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B192" t="s">
-        <v>448</v>
+        <v>402</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B193" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B194" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B195" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B196" t="s">
-        <v>449</v>
+        <v>403</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B197" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B198" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B199" t="s">
-        <v>450</v>
+        <v>404</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B200" t="s">
-        <v>299</v>
+        <v>497</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B201" t="s">
-        <v>451</v>
+        <v>498</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B202" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B203" t="s">
-        <v>452</v>
+        <v>499</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,447 +3514,455 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>453</v>
+        <v>405</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="B205" t="s">
-        <v>373</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="B206" t="s">
-        <v>374</v>
+        <v>339</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="B207" t="s">
-        <v>375</v>
+        <v>340</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="B208" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="B209" t="s">
-        <v>377</v>
+        <v>342</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="B210" t="s">
-        <v>378</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="B211" t="s">
-        <v>379</v>
+        <v>344</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="B212" t="s">
-        <v>380</v>
+        <v>345</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="B213" t="s">
-        <v>381</v>
+        <v>346</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="B214" t="s">
-        <v>382</v>
+        <v>347</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="B215" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="B216" t="s">
-        <v>384</v>
+        <v>349</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>349</v>
+        <v>500</v>
       </c>
       <c r="B217" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>317</v>
+      </c>
+      <c r="B218" t="s">
         <v>350</v>
-      </c>
-      <c r="B218" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>351</v>
+        <v>502</v>
       </c>
       <c r="B219" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>352</v>
+        <v>504</v>
       </c>
       <c r="B220" t="s">
-        <v>495</v>
+        <v>447</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="B221" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="B222" t="s">
-        <v>387</v>
+        <v>352</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
       <c r="B223" t="s">
-        <v>388</v>
+        <v>353</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
       <c r="B224" t="s">
-        <v>389</v>
+        <v>354</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="B225" t="s">
-        <v>390</v>
+        <v>355</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
       <c r="B226" t="s">
-        <v>497</v>
+        <v>449</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>359</v>
+        <v>324</v>
       </c>
       <c r="B227" t="s">
-        <v>391</v>
+        <v>356</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="B228" t="s">
-        <v>393</v>
+        <v>358</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
       <c r="B229" t="s">
-        <v>392</v>
+        <v>357</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
       <c r="B230" t="s">
-        <v>394</v>
+        <v>359</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>363</v>
+        <v>328</v>
       </c>
       <c r="B231" t="s">
-        <v>395</v>
+        <v>360</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>364</v>
+        <v>329</v>
       </c>
       <c r="B232" t="s">
-        <v>396</v>
+        <v>361</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>365</v>
+        <v>330</v>
       </c>
       <c r="B233" t="s">
-        <v>397</v>
+        <v>362</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>366</v>
+        <v>331</v>
       </c>
       <c r="B234" t="s">
-        <v>398</v>
+        <v>363</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>367</v>
+        <v>332</v>
       </c>
       <c r="B235" t="s">
-        <v>399</v>
+        <v>364</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>368</v>
+        <v>333</v>
       </c>
       <c r="B236" t="s">
-        <v>400</v>
+        <v>365</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="B237" t="s">
-        <v>401</v>
+        <v>366</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>370</v>
+        <v>335</v>
       </c>
       <c r="B238" t="s">
-        <v>402</v>
+        <v>367</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="B239" t="s">
-        <v>403</v>
+        <v>368</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="B240" t="s">
-        <v>498</v>
+        <v>450</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>454</v>
+        <v>406</v>
       </c>
       <c r="B241" t="s">
-        <v>466</v>
+        <v>418</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>455</v>
+        <v>407</v>
       </c>
       <c r="B242" t="s">
-        <v>467</v>
+        <v>419</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>456</v>
+        <v>408</v>
       </c>
       <c r="B243" t="s">
-        <v>468</v>
+        <v>420</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>457</v>
+        <v>409</v>
       </c>
       <c r="B244" t="s">
-        <v>469</v>
+        <v>421</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>458</v>
+        <v>410</v>
       </c>
       <c r="B245" t="s">
-        <v>459</v>
+        <v>411</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>460</v>
+        <v>412</v>
       </c>
       <c r="B246" t="s">
-        <v>461</v>
+        <v>413</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>462</v>
+        <v>414</v>
       </c>
       <c r="B247" t="s">
-        <v>465</v>
+        <v>417</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>463</v>
+        <v>415</v>
       </c>
       <c r="B248" t="s">
-        <v>464</v>
+        <v>416</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="B249" t="s">
-        <v>489</v>
+        <v>441</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="B250" t="s">
-        <v>490</v>
+        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="B251" t="s">
-        <v>491</v>
+        <v>443</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="B252" t="s">
-        <v>492</v>
+        <v>444</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>481</v>
+        <v>433</v>
       </c>
       <c r="B253" t="s">
-        <v>378</v>
+        <v>343</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>482</v>
+        <v>434</v>
       </c>
       <c r="B254" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>483</v>
+        <v>435</v>
       </c>
       <c r="B255" t="s">
-        <v>387</v>
+        <v>352</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>484</v>
+        <v>436</v>
       </c>
       <c r="B256" t="s">
-        <v>496</v>
+        <v>448</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>485</v>
+        <v>437</v>
       </c>
       <c r="B257" t="s">
-        <v>493</v>
+        <v>445</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>486</v>
+        <v>438</v>
       </c>
       <c r="B258" t="s">
-        <v>494</v>
+        <v>446</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>487</v>
+        <v>439</v>
       </c>
       <c r="B259" t="s">
-        <v>495</v>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>456</v>
+      </c>
+      <c r="B260" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Die englischen Texte 219-220 ausgetauscht.
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1875,8 +1875,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A236" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A249" sqref="A249"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A233" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3634,7 @@
         <v>502</v>
       </c>
       <c r="B219" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>504</v>
       </c>
       <c r="B220" t="s">
-        <v>447</v>
+        <v>503</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CopyPaste-Routinen, damit der Fehler 'Unkown Shapes' nicht mehr auftritt Bearbeitung des Titels für einzelne Report-Module geändert: Im .Title muss nun die Kennzeichnung und die Qualifier enthalten sein, Enlarge13 muss in .Alternativtext enthalten sein.
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1875,8 +1875,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A236" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A249" sqref="A249"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A194" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B216" sqref="B216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3634,7 @@
         <v>502</v>
       </c>
       <c r="B219" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>504</v>
       </c>
       <c r="B220" t="s">
-        <v>447</v>
+        <v>503</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ute Änderungen bezgl Copy/paste aufgenommen
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1875,8 +1875,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A236" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A249" sqref="A249"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A194" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B216" sqref="B216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3634,7 @@
         <v>502</v>
       </c>
       <c r="B219" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>504</v>
       </c>
       <c r="B220" t="s">
-        <v>447</v>
+        <v>503</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Report Texte ergänzt (es fehlen noch die Überschriften der Tabelle Projektliste) Routine awinImportMassenEdit clsRollen: containsName angepasst (behandelt auch einen übergebenen Nothing Wert) Methode calculateroundedKPI kann mit optionalem Parameter aufgerufen werden, so das die exakten Werte zurückgegeben werden . Das wird in Tabelle Projektliste benötigt , damit die Summen-Werte nicht unterschiedlich dargestellt werden clsPhase Methoden getRole, getCost, removeRole, removeCost hinzugefügt clsPhase: addRole, addCost geändert : wenn die Rolle /Kostenart schon existiert wird nicht eine weiter Rolle gleichen Namens hinzugefügt, sondern die Werte werden addiert Klasse Kostenarten: _allKostenarten ist wie in _allRollen eine sortierte Liste in der Inventur: jetzt kann auch eine Responsible Person mit angegeben werden Enumeration: PTImpExp um MassenEdit erweitert; die ersten fünf sind dual, das heisst es gibt Import wie Export; der Rest ist nur für Import benötigt
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="506">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -600,15 +600,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>without name</t>
-  </si>
-  <si>
-    <t>project, with &amp; vblf &amp; start- and end-marker</t>
-  </si>
-  <si>
-    <t>… does not exist in this project …</t>
-  </si>
-  <si>
     <t>Milestone Trendanalysis</t>
   </si>
   <si>
@@ -633,9 +624,6 @@
     <t>project</t>
   </si>
   <si>
-    <t>does not exist</t>
-  </si>
-  <si>
     <t xml:space="preserve">see following slides </t>
   </si>
   <si>
@@ -768,39 +756,6 @@
     <t>opportunity costs due to below-capacity</t>
   </si>
   <si>
-    <t>additional cost due to above-capacity</t>
-  </si>
-  <si>
-    <t>Budget Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result  </t>
-  </si>
-  <si>
-    <t>Bottom</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum project results (incl Risk Fee) </t>
-  </si>
-  <si>
-    <t>Result KPI</t>
-  </si>
-  <si>
-    <t>slower</t>
-  </si>
-  <si>
-    <t>faster</t>
-  </si>
-  <si>
-    <t>more expensive</t>
-  </si>
-  <si>
-    <t>less expensive</t>
-  </si>
-  <si>
     <t xml:space="preserve">no project history yet </t>
   </si>
   <si>
@@ -864,9 +819,6 @@
     <t xml:space="preserve"> milestone traffic lights </t>
   </si>
   <si>
-    <t xml:space="preserve"> missing shapes: </t>
-  </si>
-  <si>
     <t xml:space="preserve"> no milestones in project</t>
   </si>
   <si>
@@ -1164,27 +1116,6 @@
     <t>Feasibility limit</t>
   </si>
   <si>
-    <t>Potentials</t>
-  </si>
-  <si>
-    <t>Cost to date</t>
-  </si>
-  <si>
-    <t>Cost Forecast</t>
-  </si>
-  <si>
-    <t>Personnel Costs (T€)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personnel Costs are zero </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Costs are zero </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personnel Costs </t>
-  </si>
-  <si>
     <t>Other Costs</t>
   </si>
   <si>
@@ -1491,9 +1422,6 @@
     <t>additional costs due to above-capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">Personnel Needs </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Total Cost</t>
   </si>
   <si>
@@ -1534,6 +1462,81 @@
   </si>
   <si>
     <t xml:space="preserve">Details freie Kapazität </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personnel Costs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personnel Costs are zero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Costs are zero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Potentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Budget Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost to date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> does not exist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Result  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sum project results (incl Risk Fee) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> additional cost due to above-capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> opportunity costs due to below-capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Result KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> slower</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> faster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> more expensive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> less expensive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personnel Needs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personnel Costs (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> without name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> project, with &amp; vblf &amp; start- and end-marker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing shapes: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  … does not exist in this project …</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1871,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B261"/>
+  <dimension ref="A1:B262"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A236" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A261" sqref="A261"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A252" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1893,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
         <v>185</v>
@@ -1914,7 +1917,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B5" t="s">
         <v>186</v>
@@ -1922,7 +1925,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>187</v>
@@ -1973,7 +1976,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +1984,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,15 +1992,15 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>501</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2005,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2013,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2021,7 +2024,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2029,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>281</v>
+        <v>502</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,7 +2040,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2045,15 +2048,15 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="B22" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2061,7 +2064,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2069,7 +2072,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2077,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2085,7 +2088,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2093,7 +2096,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,7 +2104,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,7 +2112,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2117,7 +2120,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2125,7 +2128,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2133,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2141,7 +2144,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2149,7 +2152,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2157,15 +2160,15 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="B36" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,7 +2176,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2181,7 +2184,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2189,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2200,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2205,7 +2208,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,7 +2216,7 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2221,7 +2224,7 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,15 +2232,15 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="B45" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2248,7 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,7 +2256,7 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2261,31 +2264,31 @@
         <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="B51" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2293,23 +2296,23 @@
         <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="B53" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B54" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,7 +2320,7 @@
         <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2325,7 +2328,7 @@
         <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2333,7 +2336,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,7 +2344,7 @@
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,7 +2352,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2357,7 +2360,7 @@
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2365,7 +2368,7 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2373,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,7 +2384,7 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2392,7 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2397,7 +2400,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2405,7 +2408,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2413,7 +2416,7 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2421,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2429,7 +2432,7 @@
         <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2437,7 +2440,7 @@
         <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,7 +2448,7 @@
         <v>60</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2453,7 +2456,7 @@
         <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,7 +2464,7 @@
         <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,7 +2472,7 @@
         <v>63</v>
       </c>
       <c r="B74" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2477,7 +2480,7 @@
         <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,7 +2488,7 @@
         <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2496,7 @@
         <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,7 +2504,7 @@
         <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2512,7 @@
         <v>68</v>
       </c>
       <c r="B79" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,15 +2520,15 @@
         <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="B81" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2536,7 @@
         <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,15 +2544,15 @@
         <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="B84" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,15 +2560,15 @@
         <v>72</v>
       </c>
       <c r="B85" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="B86" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2573,7 +2576,7 @@
         <v>73</v>
       </c>
       <c r="B87" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2581,7 +2584,7 @@
         <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2592,7 @@
         <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2597,7 +2600,7 @@
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2605,7 +2608,7 @@
         <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,7 +2616,7 @@
         <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2621,7 +2624,7 @@
         <v>79</v>
       </c>
       <c r="B93" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2632,7 @@
         <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2637,7 +2640,7 @@
         <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2645,7 +2648,7 @@
         <v>82</v>
       </c>
       <c r="B96" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,7 +2656,7 @@
         <v>83</v>
       </c>
       <c r="B97" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2661,7 +2664,7 @@
         <v>84</v>
       </c>
       <c r="B98" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2669,7 +2672,7 @@
         <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2677,7 +2680,7 @@
         <v>86</v>
       </c>
       <c r="B100" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2685,7 +2688,7 @@
         <v>87</v>
       </c>
       <c r="B101" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2693,7 +2696,7 @@
         <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2701,7 +2704,7 @@
         <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2709,7 +2712,7 @@
         <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2717,7 +2720,7 @@
         <v>91</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2725,7 +2728,7 @@
         <v>92</v>
       </c>
       <c r="B106" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2733,7 +2736,7 @@
         <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2741,7 +2744,7 @@
         <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2749,7 +2752,7 @@
         <v>95</v>
       </c>
       <c r="B109" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,7 +2760,7 @@
         <v>96</v>
       </c>
       <c r="B110" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2765,7 +2768,7 @@
         <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2773,7 +2776,7 @@
         <v>98</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2781,7 +2784,7 @@
         <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2789,7 +2792,7 @@
         <v>100</v>
       </c>
       <c r="B114" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2797,7 +2800,7 @@
         <v>101</v>
       </c>
       <c r="B115" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2805,7 +2808,7 @@
         <v>102</v>
       </c>
       <c r="B116" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,15 +2816,15 @@
         <v>103</v>
       </c>
       <c r="B117" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
       <c r="B118" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2829,7 +2832,7 @@
         <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2837,7 +2840,7 @@
         <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2845,7 +2848,7 @@
         <v>106</v>
       </c>
       <c r="B121" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2853,7 +2856,7 @@
         <v>107</v>
       </c>
       <c r="B122" t="s">
-        <v>486</v>
+        <v>463</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,7 +2864,7 @@
         <v>108</v>
       </c>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,7 +2872,7 @@
         <v>109</v>
       </c>
       <c r="B124" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2877,7 +2880,7 @@
         <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2885,7 +2888,7 @@
         <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2893,7 +2896,7 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,7 +2904,7 @@
         <v>112</v>
       </c>
       <c r="B128" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2909,7 +2912,7 @@
         <v>113</v>
       </c>
       <c r="B129" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2917,7 +2920,7 @@
         <v>114</v>
       </c>
       <c r="B130" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2925,7 +2928,7 @@
         <v>115</v>
       </c>
       <c r="B131" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,7 +2936,7 @@
         <v>116</v>
       </c>
       <c r="B132" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2941,7 +2944,7 @@
         <v>117</v>
       </c>
       <c r="B133" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2949,7 +2952,7 @@
         <v>118</v>
       </c>
       <c r="B134" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2957,7 +2960,7 @@
         <v>119</v>
       </c>
       <c r="B135" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,7 +2968,7 @@
         <v>120</v>
       </c>
       <c r="B136" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,7 +2976,7 @@
         <v>121</v>
       </c>
       <c r="B137" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2981,7 +2984,7 @@
         <v>122</v>
       </c>
       <c r="B138" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2989,7 +2992,7 @@
         <v>107</v>
       </c>
       <c r="B139" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2997,7 +3000,7 @@
         <v>123</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3005,7 +3008,7 @@
         <v>124</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3013,7 +3016,7 @@
         <v>125</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3021,7 +3024,7 @@
         <v>126</v>
       </c>
       <c r="B143" t="s">
-        <v>381</v>
+        <v>484</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3029,7 +3032,7 @@
         <v>127</v>
       </c>
       <c r="B144" t="s">
-        <v>250</v>
+        <v>485</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3037,7 +3040,7 @@
         <v>128</v>
       </c>
       <c r="B145" t="s">
-        <v>382</v>
+        <v>486</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3045,7 +3048,7 @@
         <v>129</v>
       </c>
       <c r="B146" t="s">
-        <v>383</v>
+        <v>487</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3053,7 +3056,7 @@
         <v>130</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>488</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3061,7 +3064,7 @@
         <v>131</v>
       </c>
       <c r="B148" t="s">
-        <v>251</v>
+        <v>489</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3069,7 +3072,7 @@
         <v>132</v>
       </c>
       <c r="B149" t="s">
-        <v>252</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -3077,7 +3080,7 @@
         <v>133</v>
       </c>
       <c r="B150" t="s">
-        <v>253</v>
+        <v>133</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -3085,7 +3088,7 @@
         <v>134</v>
       </c>
       <c r="B151" t="s">
-        <v>254</v>
+        <v>490</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3093,7 +3096,7 @@
         <v>124</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>249</v>
+        <v>491</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3101,7 +3104,7 @@
         <v>135</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>248</v>
+        <v>492</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3109,7 +3112,7 @@
         <v>136</v>
       </c>
       <c r="B154" t="s">
-        <v>255</v>
+        <v>493</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3117,7 +3120,7 @@
         <v>137</v>
       </c>
       <c r="B155" t="s">
-        <v>256</v>
+        <v>494</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3125,7 +3128,7 @@
         <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>257</v>
+        <v>495</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3133,7 +3136,7 @@
         <v>139</v>
       </c>
       <c r="B157" t="s">
-        <v>258</v>
+        <v>496</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3141,7 +3144,7 @@
         <v>140</v>
       </c>
       <c r="B158" t="s">
-        <v>259</v>
+        <v>497</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3149,7 +3152,7 @@
         <v>141</v>
       </c>
       <c r="B159" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3157,7 +3160,7 @@
         <v>142</v>
       </c>
       <c r="B160" t="s">
-        <v>384</v>
+        <v>499</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3165,7 +3168,7 @@
         <v>143</v>
       </c>
       <c r="B161" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,7 +3176,7 @@
         <v>144</v>
       </c>
       <c r="B162" t="s">
-        <v>385</v>
+        <v>482</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3181,7 +3184,7 @@
         <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>386</v>
+        <v>483</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3189,7 +3192,7 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>387</v>
+        <v>481</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3197,7 +3200,7 @@
         <v>146</v>
       </c>
       <c r="B165" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3205,7 +3208,7 @@
         <v>147</v>
       </c>
       <c r="B166" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3213,7 +3216,7 @@
         <v>148</v>
       </c>
       <c r="B167" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3221,7 +3224,7 @@
         <v>149</v>
       </c>
       <c r="B168" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3229,7 +3232,7 @@
         <v>150</v>
       </c>
       <c r="B169" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3237,7 +3240,7 @@
         <v>151</v>
       </c>
       <c r="B170" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3245,7 +3248,7 @@
         <v>152</v>
       </c>
       <c r="B171" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3253,7 +3256,7 @@
         <v>153</v>
       </c>
       <c r="B172" t="s">
-        <v>493</v>
+        <v>469</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3261,7 +3264,7 @@
         <v>42</v>
       </c>
       <c r="B173" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -3269,15 +3272,15 @@
         <v>154</v>
       </c>
       <c r="B174" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>494</v>
+        <v>470</v>
       </c>
       <c r="B175" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -3285,7 +3288,7 @@
         <v>155</v>
       </c>
       <c r="B176" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3293,7 +3296,7 @@
         <v>156</v>
       </c>
       <c r="B177" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3301,7 +3304,7 @@
         <v>157</v>
       </c>
       <c r="B178" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3309,7 +3312,7 @@
         <v>158</v>
       </c>
       <c r="B179" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3317,7 +3320,7 @@
         <v>159</v>
       </c>
       <c r="B180" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3325,7 +3328,7 @@
         <v>160</v>
       </c>
       <c r="B181" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3333,7 +3336,7 @@
         <v>161</v>
       </c>
       <c r="B182" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3341,7 +3344,7 @@
         <v>162</v>
       </c>
       <c r="B183" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3349,7 +3352,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3357,7 +3360,7 @@
         <v>163</v>
       </c>
       <c r="B185" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3365,7 +3368,7 @@
         <v>164</v>
       </c>
       <c r="B186" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3373,7 +3376,7 @@
         <v>165</v>
       </c>
       <c r="B187" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,7 +3384,7 @@
         <v>166</v>
       </c>
       <c r="B188" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3389,7 +3392,7 @@
         <v>167</v>
       </c>
       <c r="B189" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3397,7 +3400,7 @@
         <v>168</v>
       </c>
       <c r="B190" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3405,7 +3408,7 @@
         <v>169</v>
       </c>
       <c r="B191" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3413,7 +3416,7 @@
         <v>170</v>
       </c>
       <c r="B192" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3421,7 +3424,7 @@
         <v>171</v>
       </c>
       <c r="B193" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -3429,7 +3432,7 @@
         <v>172</v>
       </c>
       <c r="B194" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3437,7 +3440,7 @@
         <v>173</v>
       </c>
       <c r="B195" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3445,7 +3448,7 @@
         <v>174</v>
       </c>
       <c r="B196" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3453,7 +3456,7 @@
         <v>175</v>
       </c>
       <c r="B197" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -3461,7 +3464,7 @@
         <v>176</v>
       </c>
       <c r="B198" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3469,7 +3472,7 @@
         <v>177</v>
       </c>
       <c r="B199" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3477,7 +3480,7 @@
         <v>178</v>
       </c>
       <c r="B200" t="s">
-        <v>495</v>
+        <v>471</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3485,7 +3488,7 @@
         <v>179</v>
       </c>
       <c r="B201" t="s">
-        <v>496</v>
+        <v>472</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3493,7 +3496,7 @@
         <v>180</v>
       </c>
       <c r="B202" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3501,7 +3504,7 @@
         <v>181</v>
       </c>
       <c r="B203" t="s">
-        <v>497</v>
+        <v>473</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3509,463 +3512,471 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="B205" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B206" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B207" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B208" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B209" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B210" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="B211" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B212" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="B213" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="B214" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B215" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B216" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>498</v>
+        <v>474</v>
       </c>
       <c r="B217" t="s">
-        <v>499</v>
+        <v>475</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="B218" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="B219" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>501</v>
+        <v>477</v>
       </c>
       <c r="B220" t="s">
-        <v>500</v>
+        <v>476</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B221" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="B222" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="B223" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="B224" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="B225" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B226" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B227" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="B228" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B229" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="B230" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="B231" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="B232" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="B233" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="B234" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B235" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="B236" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B237" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="B238" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="B239" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="B240" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="B241" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="B242" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="B243" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="B244" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="B245" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="B246" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="B247" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="B248" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B249" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="B250" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B251" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="B252" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="B253" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="B254" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="B255" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="B256" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B257" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>501</v>
+        <v>477</v>
       </c>
       <c r="B258" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="B259" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
       <c r="B260" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
       <c r="B261" t="s">
-        <v>503</v>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>504</v>
+      </c>
+      <c r="B262" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report Projektliste: letzte Zeile fett gemacht
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="522">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -603,204 +603,33 @@
     <t>Milestone Trendanalysis</t>
   </si>
   <si>
-    <t xml:space="preserve">template could not be found </t>
-  </si>
-  <si>
-    <t>no approval status reached</t>
-  </si>
-  <si>
-    <t>there is no latest version</t>
-  </si>
-  <si>
-    <t>no table in shape</t>
-  </si>
-  <si>
-    <t>to few columns in table (min 4)</t>
-  </si>
-  <si>
-    <t>table project goal has not enough rows / columns ….</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">see following slides </t>
-  </si>
-  <si>
-    <t>identical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of rows and columns does not fit to project status table </t>
-  </si>
-  <si>
-    <t>no milestones specified</t>
-  </si>
-  <si>
     <t>Budget</t>
   </si>
   <si>
-    <t>Overview Milestones</t>
-  </si>
-  <si>
-    <t>Deviations from approved version</t>
-  </si>
-  <si>
-    <t>Deviations from latest version</t>
-  </si>
-  <si>
-    <t>Budget overview</t>
-  </si>
-  <si>
-    <t>strategic Fit, Risk &amp; Influence</t>
-  </si>
-  <si>
-    <t>Error in CreatePortfolioDiagram</t>
-  </si>
-  <si>
-    <t>Error in UpdatePortfolioDiagram</t>
-  </si>
-  <si>
     <t xml:space="preserve">database connection failed &amp; vblf &amp; project history could not be loaded </t>
   </si>
   <si>
     <t xml:space="preserve"> Error in CreateBetterWorsePortfolio  </t>
   </si>
   <si>
-    <t>there are no projects with deviations greater than the allowed tolerance</t>
-  </si>
-  <si>
-    <t>Time tolerance project-end: +/-</t>
-  </si>
-  <si>
-    <t>Time tolerance next milestone: +/-</t>
-  </si>
-  <si>
-    <t>Time tolerance: +/-</t>
-  </si>
-  <si>
-    <t>Cost tolerance: +/-</t>
-  </si>
-  <si>
-    <t>Time deviation to next milestone</t>
-  </si>
-  <si>
-    <t>Time deviation project end</t>
-  </si>
-  <si>
-    <t>Cost deviation</t>
-  </si>
-  <si>
     <t>no resource needs defined</t>
   </si>
   <si>
-    <t>with limitations</t>
-  </si>
-  <si>
-    <t>fulfilled</t>
-  </si>
-  <si>
-    <t>not fulfilled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no fulfilled targets:time frame entirely in future </t>
-  </si>
-  <si>
-    <t xml:space="preserve">no forecast: time frame entirely in past </t>
-  </si>
-  <si>
-    <t xml:space="preserve">not defined: </t>
-  </si>
-  <si>
-    <t>no Phase / Role / Cost / Result / Milestone selected …</t>
-  </si>
-  <si>
-    <t>Overview Result Forecast</t>
-  </si>
-  <si>
-    <t>Overview</t>
-  </si>
-  <si>
     <t>external Resources</t>
   </si>
   <si>
-    <t>Risk Fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity incl. Ext. </t>
-  </si>
-  <si>
-    <t>not existent</t>
-  </si>
-  <si>
     <t xml:space="preserve">no table for scenario </t>
   </si>
   <si>
-    <t>no elements provided ….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shape has no table </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with cost </t>
-  </si>
-  <si>
-    <t>no projects in given time frame</t>
-  </si>
-  <si>
-    <t>no phases provided …</t>
-  </si>
-  <si>
-    <t>no current projects in given time frame …</t>
-  </si>
-  <si>
     <t>opportunity costs due to below-capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">no project history yet </t>
-  </si>
-  <si>
     <t>Result (Forecast)</t>
   </si>
   <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>planned</t>
-  </si>
-  <si>
-    <t>actual</t>
-  </si>
-  <si>
-    <t>project not yet started …</t>
-  </si>
-  <si>
-    <t>project has already ended</t>
-  </si>
-  <si>
-    <t>no latest version</t>
-  </si>
-  <si>
-    <t>Error in min-/max-calculation</t>
-  </si>
-  <si>
-    <t>actual values</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
     <t xml:space="preserve"> not possible …</t>
   </si>
   <si>
-    <t>clarification needed, whether to consider past or future …</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Dep.) </t>
   </si>
   <si>
@@ -1080,12 +909,6 @@
     <t>Projectphases</t>
   </si>
   <si>
-    <t>Forecast</t>
-  </si>
-  <si>
-    <t>Reporting Periods</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (approved version)</t>
   </si>
   <si>
@@ -1098,78 +921,15 @@
     <t xml:space="preserve"> Risk Fee</t>
   </si>
   <si>
-    <t>above Capacity</t>
-  </si>
-  <si>
-    <t>below Capacity</t>
-  </si>
-  <si>
-    <t>Fulfillment expected</t>
-  </si>
-  <si>
-    <t>Fulfillment with uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fulfillment with high risks </t>
-  </si>
-  <si>
-    <t>Feasibility limit</t>
-  </si>
-  <si>
     <t>Other Costs</t>
   </si>
   <si>
     <t xml:space="preserve">sum Other Cost is zero </t>
   </si>
   <si>
-    <t xml:space="preserve">Total Cost is zero </t>
-  </si>
-  <si>
-    <t>strategic Fit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost of Risk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">target / actual Personnel Cost not possible </t>
-  </si>
-  <si>
-    <t xml:space="preserve">target / actual Other Cost not possible </t>
-  </si>
-  <si>
-    <t xml:space="preserve">target / actual Total Cost not possible </t>
-  </si>
-  <si>
-    <t xml:space="preserve">no approved version </t>
-  </si>
-  <si>
-    <t>min/max Personnel Cost (T€)</t>
-  </si>
-  <si>
-    <t>target-/actual Personnel Cost (T€)</t>
-  </si>
-  <si>
-    <t>min/max Other Cost (T€)</t>
-  </si>
-  <si>
-    <t>target-/actual Other Cost (T€)</t>
-  </si>
-  <si>
-    <t>min/max Total Cost (T€)</t>
-  </si>
-  <si>
-    <t>target-/actual Total Cost (T€)</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
-    <t xml:space="preserve">target-/actual Cost </t>
-  </si>
-  <si>
     <t>Termine Phasen</t>
   </si>
   <si>
@@ -1218,27 +978,6 @@
     <t xml:space="preserve">Risk </t>
   </si>
   <si>
-    <t xml:space="preserve">all projects with milestone  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with phase  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with role  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with milestones  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with phases  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with roles  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">all projects with costs  </t>
-  </si>
-  <si>
     <t>Prognose Ergebniskennzahl</t>
   </si>
   <si>
@@ -1266,9 +1005,6 @@
     <t>Auslastungs-Übersicht</t>
   </si>
   <si>
-    <t xml:space="preserve">Phase </t>
-  </si>
-  <si>
     <t>Forecast Result</t>
   </si>
   <si>
@@ -1320,24 +1056,15 @@
     <t>Internal Capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">please use another template - projects do not fit to one page ???  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> zu diesem Projekt gibt es noch keine Trend-Analyse, &amp; vblf &amp; da es noch nicht begonnen hat</t>
   </si>
   <si>
-    <t xml:space="preserve">project template does not exist  </t>
-  </si>
-  <si>
     <t xml:space="preserve">  does not exist</t>
   </si>
   <si>
     <t xml:space="preserve"> Tabelle Projektänderungen hat evtl unzulässige Anzahl Zeilen / Spalten …</t>
   </si>
   <si>
-    <t xml:space="preserve">table project changes with wrong number of rows / columns </t>
-  </si>
-  <si>
     <t>there is no trend for that project '</t>
   </si>
   <si>
@@ -1389,60 +1116,24 @@
     <t xml:space="preserve"> Projects without latest version</t>
   </si>
   <si>
-    <t>no achieved targets …</t>
-  </si>
-  <si>
-    <t>no future targets defined …</t>
-  </si>
-  <si>
-    <t>no achieved nor future targets …</t>
-  </si>
-  <si>
     <t xml:space="preserve"> internal </t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity utilization </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Kapazität inkl. Externe</t>
   </si>
   <si>
-    <t xml:space="preserve">Milestone </t>
-  </si>
-  <si>
     <t xml:space="preserve"> not existent</t>
   </si>
   <si>
-    <t xml:space="preserve">no time frame provided in table </t>
-  </si>
-  <si>
     <t xml:space="preserve"> please provide time frame …</t>
   </si>
   <si>
-    <t>additional costs due to above-capacity</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Total Cost</t>
   </si>
   <si>
-    <t xml:space="preserve">history strategic fit &amp; risk: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">History of KPI </t>
-  </si>
-  <si>
     <t>progn. Ergebnis</t>
   </si>
   <si>
-    <t xml:space="preserve">Role </t>
-  </si>
-  <si>
-    <t xml:space="preserve">target-/actual Role Needs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost </t>
-  </si>
-  <si>
     <t xml:space="preserve">Übersicht Auslastung </t>
   </si>
   <si>
@@ -1537,6 +1228,363 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> please use another template - projects do not fit to one page ???  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> project template does not exist  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> template could not be found </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no approval status reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> there is no latest version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no table in shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to few columns in table (min 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> table project goal has not enough rows / columns ….</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> see following slides </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> identical</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> table project changes with wrong number of rows / columns </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> number of rows and columns does not fit to project status table </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no milestones specified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reporting Periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deviations from latest version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deviations from approved version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Budget overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> strategic Fit, Risk &amp; Influence</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error in CreatePortfolioDiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error in UpdatePortfolioDiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> there are no projects with deviations greater than the allowed tolerance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time tolerance project-end: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time tolerance next milestone: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time tolerance: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost tolerance: +/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time deviation to next milestone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time deviation project end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capacity utilization </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> above Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> below Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no resource needs defined</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fulfilled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> with limitations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> not fulfilled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no fulfilled targets:time frame entirely in future </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fulfillment expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fulfillment with uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fulfillment with high risks </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no forecast: time frame entirely in past </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clarification needed, whether to consider past or future …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no achieved targets …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no future targets defined …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no achieved nor future targets …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> not defined: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no Phase / Role / Cost / Result / Milestone selected …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Overview Result Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Capacity incl. Ext. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feasibility limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Milestone </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no time frame provided in table </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no elements provided ….</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shape has no table </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with milestone  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with phase  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with role  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with cost </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with milestones  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with phases  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with roles  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all projects with costs  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no projects in given time frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no phases provided …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no current projects in given time frame …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> additional costs due to above-capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Cost is zero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> history strategic fit &amp; risk: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> strategic Fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no project history yet </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> History of KPI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost of Risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> planned</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> project not yet started …</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> project has already ended</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target / actual Personnel Cost not possible </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target / actual Other Cost not possible </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target / actual Total Cost not possible </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no approved version </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no latest version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error in min-/max-calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> min/max Personnel Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target-/actual Personnel Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> min/max Other Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target-/actual Other Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> min/max Total Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target-/actual Total Cost (T€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> actual values</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Role </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target-/actual Role Needs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cost </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> target-/actual Cost </t>
+  </si>
+  <si>
+    <t>Projekt-Name</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>Budget &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>P.-Bedarfe &amp; vblf &amp; (PT)</t>
+  </si>
+  <si>
+    <t>E.-Kosten &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Stand vom</t>
+  </si>
+  <si>
+    <t>Project-Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>P.-Needs &amp; vblf &amp; (FTE)</t>
+  </si>
+  <si>
+    <t>Ext.-Cost &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Ergebnis &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Result &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Version from</t>
+  </si>
+  <si>
+    <t>rT&amp; vblf &amp;(Tage)</t>
+  </si>
+  <si>
+    <t>rE&amp; vblf &amp;(T€)</t>
+  </si>
+  <si>
+    <t>rL&amp; vblf &amp;(Anz.)</t>
+  </si>
+  <si>
+    <t>rT&amp; vblf &amp;(days)</t>
+  </si>
+  <si>
+    <t>rD&amp; vblf &amp;(Deliv.)</t>
   </si>
 </sst>
 </file>
@@ -1871,16 +1919,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B262"/>
+  <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A252" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A241" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="122.42578125" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,7 +1941,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>426</v>
+        <v>338</v>
       </c>
       <c r="B2" t="s">
         <v>185</v>
@@ -1917,7 +1965,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>339</v>
       </c>
       <c r="B5" t="s">
         <v>186</v>
@@ -1925,7 +1973,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>428</v>
+        <v>340</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>187</v>
@@ -1976,7 +2024,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,7 +2032,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,15 +2040,15 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>500</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>429</v>
+        <v>341</v>
       </c>
       <c r="B15" t="s">
-        <v>501</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2056,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2016,7 +2064,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2024,7 +2072,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2032,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>502</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>503</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2053,10 +2101,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>434</v>
+        <v>345</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2112,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2120,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
+        <v>406</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,7 +2144,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>407</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2104,7 +2152,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,7 +2160,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2168,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>410</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2176,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>411</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2184,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>436</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2192,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2200,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,15 +2208,15 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>267</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>437</v>
+        <v>347</v>
       </c>
       <c r="B36" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2224,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>415</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>353</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2240,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>439</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2248,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2208,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>354</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2216,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>440</v>
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2272,7 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>441</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,15 +2280,15 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>442</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>443</v>
+        <v>352</v>
       </c>
       <c r="B45" t="s">
-        <v>269</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2248,7 +2296,7 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2304,7 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>355</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,31 +2312,31 @@
         <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>444</v>
+        <v>353</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>447</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>445</v>
+        <v>354</v>
       </c>
       <c r="B51" t="s">
-        <v>448</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,23 +2344,23 @@
         <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>365</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>446</v>
+        <v>355</v>
       </c>
       <c r="B53" t="s">
-        <v>449</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
       <c r="B54" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2320,7 +2368,7 @@
         <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>356</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2328,7 +2376,7 @@
         <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>357</v>
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2336,7 +2384,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>358</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2344,7 +2392,7 @@
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2352,7 +2400,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>273</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2360,7 +2408,7 @@
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,7 +2416,7 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>275</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2376,7 +2424,7 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>276</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2384,7 +2432,7 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>277</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2392,7 +2440,7 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2448,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>279</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,7 +2456,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2416,7 +2464,7 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>207</v>
+        <v>420</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,7 +2472,7 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>421</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,7 +2480,7 @@
         <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>210</v>
+        <v>422</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2440,7 +2488,7 @@
         <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2448,7 +2496,7 @@
         <v>60</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2504,7 @@
         <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2464,7 +2512,7 @@
         <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>281</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2472,7 +2520,7 @@
         <v>63</v>
       </c>
       <c r="B74" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2480,7 +2528,7 @@
         <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>283</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2488,7 +2536,7 @@
         <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>284</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2496,7 +2544,7 @@
         <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>285</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2504,7 +2552,7 @@
         <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>424</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2512,7 +2560,7 @@
         <v>68</v>
       </c>
       <c r="B79" t="s">
-        <v>450</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2520,15 +2568,15 @@
         <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>451</v>
+        <v>360</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="B81" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2536,7 +2584,7 @@
         <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2544,15 +2592,15 @@
         <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>425</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>452</v>
+        <v>361</v>
       </c>
       <c r="B84" t="s">
-        <v>216</v>
+        <v>426</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2560,15 +2608,15 @@
         <v>72</v>
       </c>
       <c r="B85" t="s">
-        <v>217</v>
+        <v>427</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>453</v>
+        <v>362</v>
       </c>
       <c r="B86" t="s">
-        <v>218</v>
+        <v>428</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2576,7 +2624,7 @@
         <v>73</v>
       </c>
       <c r="B87" t="s">
-        <v>219</v>
+        <v>429</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2584,7 +2632,7 @@
         <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>220</v>
+        <v>430</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2592,7 +2640,7 @@
         <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>431</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2600,7 +2648,7 @@
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>222</v>
+        <v>432</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2608,7 +2656,7 @@
         <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>454</v>
+        <v>363</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2616,7 +2664,7 @@
         <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>455</v>
+        <v>364</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,7 +2672,7 @@
         <v>79</v>
       </c>
       <c r="B93" t="s">
-        <v>460</v>
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +2680,7 @@
         <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>359</v>
+        <v>434</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2688,7 @@
         <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>360</v>
+        <v>435</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2696,7 @@
         <v>82</v>
       </c>
       <c r="B96" t="s">
-        <v>223</v>
+        <v>436</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2656,7 +2704,7 @@
         <v>83</v>
       </c>
       <c r="B97" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2664,7 +2712,7 @@
         <v>84</v>
       </c>
       <c r="B98" t="s">
-        <v>225</v>
+        <v>437</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2672,7 +2720,7 @@
         <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>224</v>
+        <v>438</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2680,7 +2728,7 @@
         <v>86</v>
       </c>
       <c r="B100" t="s">
-        <v>226</v>
+        <v>439</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2688,7 +2736,7 @@
         <v>87</v>
       </c>
       <c r="B101" t="s">
-        <v>227</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,7 +2744,7 @@
         <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>361</v>
+        <v>441</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2704,7 +2752,7 @@
         <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>362</v>
+        <v>442</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,7 +2760,7 @@
         <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2720,7 +2768,7 @@
         <v>91</v>
       </c>
       <c r="B105" t="s">
-        <v>228</v>
+        <v>444</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2728,7 +2776,7 @@
         <v>92</v>
       </c>
       <c r="B106" t="s">
-        <v>259</v>
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2736,7 +2784,7 @@
         <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,7 +2792,7 @@
         <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2752,7 +2800,7 @@
         <v>95</v>
       </c>
       <c r="B109" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2760,7 +2808,7 @@
         <v>96</v>
       </c>
       <c r="B110" t="s">
-        <v>415</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2768,7 +2816,7 @@
         <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>229</v>
+        <v>449</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2776,7 +2824,7 @@
         <v>98</v>
       </c>
       <c r="B112" t="s">
-        <v>230</v>
+        <v>450</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,7 +2832,7 @@
         <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>231</v>
+        <v>451</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2792,7 +2840,7 @@
         <v>100</v>
       </c>
       <c r="B114" t="s">
-        <v>232</v>
+        <v>452</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2800,7 +2848,7 @@
         <v>101</v>
       </c>
       <c r="B115" t="s">
-        <v>459</v>
+        <v>365</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2808,7 +2856,7 @@
         <v>102</v>
       </c>
       <c r="B116" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2816,15 +2864,15 @@
         <v>103</v>
       </c>
       <c r="B117" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>461</v>
+        <v>366</v>
       </c>
       <c r="B118" t="s">
-        <v>235</v>
+        <v>453</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2832,7 +2880,7 @@
         <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>364</v>
+        <v>454</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2840,7 +2888,7 @@
         <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,7 +2896,7 @@
         <v>106</v>
       </c>
       <c r="B121" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2856,7 +2904,7 @@
         <v>107</v>
       </c>
       <c r="B122" t="s">
-        <v>463</v>
+        <v>367</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2864,7 +2912,7 @@
         <v>108</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2872,7 +2920,7 @@
         <v>109</v>
       </c>
       <c r="B124" t="s">
-        <v>286</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2880,7 +2928,7 @@
         <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2888,7 +2936,7 @@
         <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>238</v>
+        <v>457</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2896,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>239</v>
+        <v>458</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2904,7 +2952,7 @@
         <v>112</v>
       </c>
       <c r="B128" t="s">
-        <v>399</v>
+        <v>459</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2912,7 +2960,7 @@
         <v>113</v>
       </c>
       <c r="B129" t="s">
-        <v>400</v>
+        <v>460</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2920,7 +2968,7 @@
         <v>114</v>
       </c>
       <c r="B130" t="s">
-        <v>401</v>
+        <v>461</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2928,7 +2976,7 @@
         <v>115</v>
       </c>
       <c r="B131" t="s">
-        <v>240</v>
+        <v>462</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2936,7 +2984,7 @@
         <v>116</v>
       </c>
       <c r="B132" t="s">
-        <v>402</v>
+        <v>463</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,7 +2992,7 @@
         <v>117</v>
       </c>
       <c r="B133" t="s">
-        <v>403</v>
+        <v>464</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,7 +3000,7 @@
         <v>118</v>
       </c>
       <c r="B134" t="s">
-        <v>404</v>
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2960,7 +3008,7 @@
         <v>119</v>
       </c>
       <c r="B135" t="s">
-        <v>405</v>
+        <v>466</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2968,7 +3016,7 @@
         <v>120</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
+        <v>467</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +3024,7 @@
         <v>121</v>
       </c>
       <c r="B137" t="s">
-        <v>465</v>
+        <v>368</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +3032,7 @@
         <v>122</v>
       </c>
       <c r="B138" t="s">
-        <v>242</v>
+        <v>468</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,7 +3040,7 @@
         <v>107</v>
       </c>
       <c r="B139" t="s">
-        <v>236</v>
+        <v>367</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +3048,7 @@
         <v>123</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>469</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3056,7 @@
         <v>124</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3064,7 @@
         <v>125</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3072,7 @@
         <v>126</v>
       </c>
       <c r="B143" t="s">
-        <v>484</v>
+        <v>381</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3080,7 @@
         <v>127</v>
       </c>
       <c r="B144" t="s">
-        <v>485</v>
+        <v>382</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3088,7 @@
         <v>128</v>
       </c>
       <c r="B145" t="s">
-        <v>486</v>
+        <v>383</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3096,7 @@
         <v>129</v>
       </c>
       <c r="B146" t="s">
-        <v>487</v>
+        <v>384</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3104,7 @@
         <v>130</v>
       </c>
       <c r="B147" t="s">
-        <v>488</v>
+        <v>385</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3112,7 @@
         <v>131</v>
       </c>
       <c r="B148" t="s">
-        <v>489</v>
+        <v>386</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3136,7 @@
         <v>134</v>
       </c>
       <c r="B151" t="s">
-        <v>490</v>
+        <v>387</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3144,7 @@
         <v>124</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>491</v>
+        <v>388</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3152,7 @@
         <v>135</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>492</v>
+        <v>389</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3160,7 @@
         <v>136</v>
       </c>
       <c r="B154" t="s">
-        <v>493</v>
+        <v>390</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3168,7 @@
         <v>137</v>
       </c>
       <c r="B155" t="s">
-        <v>494</v>
+        <v>391</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3128,7 +3176,7 @@
         <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>495</v>
+        <v>392</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3184,7 @@
         <v>139</v>
       </c>
       <c r="B157" t="s">
-        <v>496</v>
+        <v>393</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3192,7 @@
         <v>140</v>
       </c>
       <c r="B158" t="s">
-        <v>497</v>
+        <v>394</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3200,7 @@
         <v>141</v>
       </c>
       <c r="B159" t="s">
-        <v>498</v>
+        <v>395</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3208,7 @@
         <v>142</v>
       </c>
       <c r="B160" t="s">
-        <v>499</v>
+        <v>396</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3216,7 @@
         <v>143</v>
       </c>
       <c r="B161" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3224,7 @@
         <v>144</v>
       </c>
       <c r="B162" t="s">
-        <v>482</v>
+        <v>379</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3232,7 @@
         <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>483</v>
+        <v>380</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3192,7 +3240,7 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>481</v>
+        <v>378</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3200,7 +3248,7 @@
         <v>146</v>
       </c>
       <c r="B165" t="s">
-        <v>365</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,7 +3256,7 @@
         <v>147</v>
       </c>
       <c r="B166" t="s">
-        <v>467</v>
+        <v>369</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3216,7 +3264,7 @@
         <v>148</v>
       </c>
       <c r="B167" t="s">
-        <v>366</v>
+        <v>301</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3224,7 +3272,7 @@
         <v>149</v>
       </c>
       <c r="B168" t="s">
-        <v>367</v>
+        <v>471</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3232,7 +3280,7 @@
         <v>150</v>
       </c>
       <c r="B169" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,7 +3288,7 @@
         <v>151</v>
       </c>
       <c r="B170" t="s">
-        <v>368</v>
+        <v>473</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3248,7 +3296,7 @@
         <v>152</v>
       </c>
       <c r="B171" t="s">
-        <v>245</v>
+        <v>474</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3256,7 +3304,7 @@
         <v>153</v>
       </c>
       <c r="B172" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3264,7 +3312,7 @@
         <v>42</v>
       </c>
       <c r="B173" t="s">
-        <v>205</v>
+        <v>42</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -3272,15 +3320,15 @@
         <v>154</v>
       </c>
       <c r="B174" t="s">
-        <v>369</v>
+        <v>476</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>470</v>
+        <v>370</v>
       </c>
       <c r="B175" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3336,7 @@
         <v>155</v>
       </c>
       <c r="B176" t="s">
-        <v>247</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3344,7 @@
         <v>156</v>
       </c>
       <c r="B177" t="s">
-        <v>248</v>
+        <v>478</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3352,7 @@
         <v>157</v>
       </c>
       <c r="B178" t="s">
-        <v>249</v>
+        <v>479</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3312,7 +3360,7 @@
         <v>158</v>
       </c>
       <c r="B179" t="s">
-        <v>250</v>
+        <v>480</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,7 +3368,7 @@
         <v>159</v>
       </c>
       <c r="B180" t="s">
-        <v>251</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3328,7 +3376,7 @@
         <v>160</v>
       </c>
       <c r="B181" t="s">
-        <v>370</v>
+        <v>482</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3336,7 +3384,7 @@
         <v>161</v>
       </c>
       <c r="B182" t="s">
-        <v>371</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3344,7 +3392,7 @@
         <v>162</v>
       </c>
       <c r="B183" t="s">
-        <v>372</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3352,7 +3400,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>373</v>
+        <v>485</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3360,7 +3408,7 @@
         <v>163</v>
       </c>
       <c r="B185" t="s">
-        <v>252</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,7 +3416,7 @@
         <v>164</v>
       </c>
       <c r="B186" t="s">
-        <v>253</v>
+        <v>487</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3376,7 +3424,7 @@
         <v>165</v>
       </c>
       <c r="B187" t="s">
-        <v>374</v>
+        <v>488</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3384,7 +3432,7 @@
         <v>166</v>
       </c>
       <c r="B188" t="s">
-        <v>375</v>
+        <v>489</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3392,7 +3440,7 @@
         <v>167</v>
       </c>
       <c r="B189" t="s">
-        <v>376</v>
+        <v>490</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3400,7 +3448,7 @@
         <v>168</v>
       </c>
       <c r="B190" t="s">
-        <v>377</v>
+        <v>491</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3408,7 +3456,7 @@
         <v>169</v>
       </c>
       <c r="B191" t="s">
-        <v>378</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3416,7 +3464,7 @@
         <v>170</v>
       </c>
       <c r="B192" t="s">
-        <v>379</v>
+        <v>493</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3424,7 +3472,7 @@
         <v>171</v>
       </c>
       <c r="B193" t="s">
-        <v>288</v>
+        <v>231</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -3432,7 +3480,7 @@
         <v>172</v>
       </c>
       <c r="B194" t="s">
-        <v>254</v>
+        <v>494</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3440,7 +3488,7 @@
         <v>173</v>
       </c>
       <c r="B195" t="s">
-        <v>255</v>
+        <v>495</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3448,7 +3496,7 @@
         <v>174</v>
       </c>
       <c r="B196" t="s">
-        <v>380</v>
+        <v>496</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,7 +3504,7 @@
         <v>175</v>
       </c>
       <c r="B197" t="s">
-        <v>256</v>
+        <v>497</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -3464,7 +3512,7 @@
         <v>176</v>
       </c>
       <c r="B198" t="s">
-        <v>257</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3472,7 +3520,7 @@
         <v>177</v>
       </c>
       <c r="B199" t="s">
-        <v>381</v>
+        <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3480,7 +3528,7 @@
         <v>178</v>
       </c>
       <c r="B200" t="s">
-        <v>471</v>
+        <v>499</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3488,7 +3536,7 @@
         <v>179</v>
       </c>
       <c r="B201" t="s">
-        <v>472</v>
+        <v>500</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,7 +3544,7 @@
         <v>180</v>
       </c>
       <c r="B202" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3504,7 +3552,7 @@
         <v>181</v>
       </c>
       <c r="B203" t="s">
-        <v>473</v>
+        <v>501</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3512,471 +3560,559 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>382</v>
+        <v>502</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="B205" t="s">
-        <v>322</v>
+        <v>265</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>290</v>
+        <v>233</v>
       </c>
       <c r="B206" t="s">
-        <v>323</v>
+        <v>266</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>291</v>
+        <v>234</v>
       </c>
       <c r="B207" t="s">
-        <v>324</v>
+        <v>267</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>292</v>
+        <v>235</v>
       </c>
       <c r="B208" t="s">
-        <v>325</v>
+        <v>268</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>293</v>
+        <v>236</v>
       </c>
       <c r="B209" t="s">
-        <v>326</v>
+        <v>269</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B210" t="s">
-        <v>327</v>
+        <v>270</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>295</v>
+        <v>238</v>
       </c>
       <c r="B211" t="s">
-        <v>328</v>
+        <v>271</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>296</v>
+        <v>239</v>
       </c>
       <c r="B212" t="s">
-        <v>329</v>
+        <v>272</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>297</v>
+        <v>240</v>
       </c>
       <c r="B213" t="s">
-        <v>330</v>
+        <v>273</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>298</v>
+        <v>241</v>
       </c>
       <c r="B214" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>299</v>
+        <v>242</v>
       </c>
       <c r="B215" t="s">
-        <v>332</v>
+        <v>275</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="B216" t="s">
-        <v>333</v>
+        <v>276</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>474</v>
+        <v>371</v>
       </c>
       <c r="B217" t="s">
-        <v>475</v>
+        <v>372</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
       <c r="B218" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>480</v>
+        <v>377</v>
       </c>
       <c r="B219" t="s">
-        <v>422</v>
+        <v>334</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>477</v>
+        <v>374</v>
       </c>
       <c r="B220" t="s">
-        <v>476</v>
+        <v>373</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>302</v>
+        <v>245</v>
       </c>
       <c r="B221" t="s">
-        <v>335</v>
+        <v>278</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="B222" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="B223" t="s">
-        <v>337</v>
+        <v>280</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
       <c r="B224" t="s">
-        <v>338</v>
+        <v>281</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
       <c r="B225" t="s">
-        <v>339</v>
+        <v>282</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>307</v>
+        <v>250</v>
       </c>
       <c r="B226" t="s">
-        <v>424</v>
+        <v>336</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
       <c r="B227" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>309</v>
+        <v>252</v>
       </c>
       <c r="B228" t="s">
-        <v>342</v>
+        <v>285</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="B229" t="s">
-        <v>341</v>
+        <v>284</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>311</v>
+        <v>254</v>
       </c>
       <c r="B230" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>312</v>
+        <v>255</v>
       </c>
       <c r="B231" t="s">
-        <v>344</v>
+        <v>287</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>313</v>
+        <v>256</v>
       </c>
       <c r="B232" t="s">
-        <v>345</v>
+        <v>288</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>314</v>
+        <v>257</v>
       </c>
       <c r="B233" t="s">
-        <v>346</v>
+        <v>289</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>315</v>
+        <v>258</v>
       </c>
       <c r="B234" t="s">
-        <v>347</v>
+        <v>290</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>316</v>
+        <v>259</v>
       </c>
       <c r="B235" t="s">
-        <v>348</v>
+        <v>291</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="B236" t="s">
-        <v>349</v>
+        <v>292</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>318</v>
+        <v>261</v>
       </c>
       <c r="B237" t="s">
-        <v>350</v>
+        <v>293</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>319</v>
+        <v>262</v>
       </c>
       <c r="B238" t="s">
-        <v>351</v>
+        <v>294</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>320</v>
+        <v>263</v>
       </c>
       <c r="B239" t="s">
-        <v>352</v>
+        <v>295</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>321</v>
+        <v>264</v>
       </c>
       <c r="B240" t="s">
-        <v>425</v>
+        <v>337</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>383</v>
+        <v>303</v>
       </c>
       <c r="B241" t="s">
-        <v>395</v>
+        <v>315</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>384</v>
+        <v>304</v>
       </c>
       <c r="B242" t="s">
-        <v>396</v>
+        <v>316</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>385</v>
+        <v>305</v>
       </c>
       <c r="B243" t="s">
-        <v>397</v>
+        <v>317</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>386</v>
+        <v>306</v>
       </c>
       <c r="B244" t="s">
-        <v>398</v>
+        <v>318</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>387</v>
+        <v>307</v>
       </c>
       <c r="B245" t="s">
-        <v>388</v>
+        <v>308</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
       <c r="B246" t="s">
-        <v>390</v>
+        <v>310</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>391</v>
+        <v>311</v>
       </c>
       <c r="B247" t="s">
-        <v>394</v>
+        <v>314</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>392</v>
+        <v>312</v>
       </c>
       <c r="B248" t="s">
-        <v>393</v>
+        <v>313</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>406</v>
+        <v>319</v>
       </c>
       <c r="B249" t="s">
-        <v>416</v>
+        <v>328</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>407</v>
+        <v>320</v>
       </c>
       <c r="B250" t="s">
-        <v>417</v>
+        <v>329</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>408</v>
+        <v>321</v>
       </c>
       <c r="B251" t="s">
-        <v>418</v>
+        <v>330</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>409</v>
+        <v>322</v>
       </c>
       <c r="B252" t="s">
-        <v>419</v>
+        <v>331</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>410</v>
+        <v>323</v>
       </c>
       <c r="B253" t="s">
-        <v>327</v>
+        <v>270</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>411</v>
+        <v>324</v>
       </c>
       <c r="B254" t="s">
-        <v>335</v>
+        <v>278</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>412</v>
+        <v>325</v>
       </c>
       <c r="B255" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>413</v>
+        <v>326</v>
       </c>
       <c r="B256" t="s">
-        <v>423</v>
+        <v>335</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>414</v>
+        <v>327</v>
       </c>
       <c r="B257" t="s">
-        <v>420</v>
+        <v>332</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>477</v>
+        <v>374</v>
       </c>
       <c r="B258" t="s">
-        <v>421</v>
+        <v>333</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>480</v>
+        <v>377</v>
       </c>
       <c r="B259" t="s">
-        <v>422</v>
+        <v>334</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="B260" t="s">
-        <v>432</v>
+        <v>344</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>478</v>
+        <v>375</v>
       </c>
       <c r="B261" t="s">
-        <v>479</v>
+        <v>376</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
+        <v>401</v>
+      </c>
+      <c r="B262" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>503</v>
+      </c>
+      <c r="B263" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
         <v>504</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B264" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>505</v>
+      </c>
+      <c r="B265" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>506</v>
+      </c>
+      <c r="B266" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>507</v>
+      </c>
+      <c r="B267" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>508</v>
+      </c>
+      <c r="B268" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>514</v>
+      </c>
+      <c r="B269" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>518</v>
+      </c>
+      <c r="B270" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>517</v>
+      </c>
+      <c r="B271" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>519</v>
+      </c>
+      <c r="B272" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>509</v>
+      </c>
+      <c r="B273" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Variable menuCult (analog zu repCúlt) eingeführt in der FrmHierarchy wird jetzt immer die Stufe 50 als Default gesucht ...
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1910,7 +1910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1921,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A241" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A255" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A174" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
englisch Menu und Formualr Einträge weiter vorangetrieben ( noch nicht vollständig !)
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1910,7 +1910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1921,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A255" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A174" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A143" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A163" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SmartPPT auf englisch angepasst
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -192,9 +192,6 @@
     <t xml:space="preserve"> Abweichungen zur Beauftragung</t>
   </si>
   <si>
-    <t xml:space="preserve"> Budget Übersicht</t>
-  </si>
-  <si>
     <t xml:space="preserve"> strategischer Fit, Risiko &amp; Ausstrahlung</t>
   </si>
   <si>
@@ -735,9 +732,6 @@
     <t>Ergebnis Verbesserungspotential</t>
   </si>
   <si>
-    <t>Übersicht Budget</t>
-  </si>
-  <si>
     <t>Ergebnis</t>
   </si>
   <si>
@@ -834,9 +828,6 @@
     <t>Improvement Potential for Result</t>
   </si>
   <si>
-    <t>Overview Budget</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -852,9 +843,6 @@
     <t>Overview Better/Worse</t>
   </si>
   <si>
-    <t xml:space="preserve"> (FTE)</t>
-  </si>
-  <si>
     <t>Current Target Achievements</t>
   </si>
   <si>
@@ -1284,9 +1272,6 @@
     <t xml:space="preserve"> Deviations from approved version</t>
   </si>
   <si>
-    <t xml:space="preserve"> Budget overview</t>
-  </si>
-  <si>
     <t xml:space="preserve"> strategic Fit, Risk &amp; Influence</t>
   </si>
   <si>
@@ -1557,9 +1542,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>P.-Needs &amp; vblf &amp; (FTE)</t>
-  </si>
-  <si>
     <t>Ext.-Cost &amp; vblf &amp; (T€)</t>
   </si>
   <si>
@@ -1585,6 +1567,24 @@
   </si>
   <si>
     <t>rD&amp; vblf &amp;(Deliv.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Budget / Ergebnis Übersicht</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Budget / Result overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (PD)</t>
+  </si>
+  <si>
+    <t>P.-Needs &amp; vblf &amp; (PD)</t>
+  </si>
+  <si>
+    <t>Overview Budget / Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget / Ergebnis Übersicht </t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1921,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A143" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A163" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A151" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,15 +1936,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1960,23 +1960,23 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2016,7 +2016,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2024,7 +2024,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,15 +2040,15 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B15" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2072,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,15 +2096,15 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,7 +2112,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2168,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2192,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2208,15 +2208,15 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B36" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,15 +2280,15 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2312,55 +2312,55 @@
         <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B51" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B53" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
         <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,7 +2432,7 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2464,479 +2464,479 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>516</v>
       </c>
       <c r="B68" t="s">
-        <v>421</v>
+        <v>517</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B83" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B84" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B85" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B86" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B87" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B88" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B90" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B92" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B96" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B101" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B104" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B106" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B108" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B109" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B110" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B111" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B112" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B113" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B114" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B115" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B116" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B117" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B118" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B121" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,295 +2944,295 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B128" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B129" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B130" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B131" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B132" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B133" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B134" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B135" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B136" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B137" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B138" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B139" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B140" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B144" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B145" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B146" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B147" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B148" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B151" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B154" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B155" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B158" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B159" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B160" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B161" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B162" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B163" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,71 +3240,71 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B165" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B166" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B167" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B168" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B169" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B170" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B171" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B172" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3317,82 +3317,82 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B174" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B175" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B176" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B177" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B178" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B179" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B180" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B181" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B182" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B183" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3400,159 +3400,159 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B185" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B186" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B187" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B188" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B190" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B191" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B192" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B193" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B194" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B195" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B196" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B197" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B198" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B199" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B200" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B201" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B202" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B203" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3560,559 +3560,559 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B205" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B206" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B207" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B208" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B209" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B210" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>238</v>
+        <v>521</v>
       </c>
       <c r="B211" t="s">
-        <v>271</v>
+        <v>520</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B212" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B213" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B214" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B215" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B216" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B217" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B218" t="s">
-        <v>277</v>
+        <v>518</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B219" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B220" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B221" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B222" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B223" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B224" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B225" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B226" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B227" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B228" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B229" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B230" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B231" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B232" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B233" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B234" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B235" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B236" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B237" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B238" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B239" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B240" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B241" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B242" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B243" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B244" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B245" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B246" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B247" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B248" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B249" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B250" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B251" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B252" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B253" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B254" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B255" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B256" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B257" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B258" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B259" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B260" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B261" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B262" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B263" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="B264" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="B265" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B266" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B267" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B268" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="B269" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="B270" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B271" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B272" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B273" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mass-Edit Ressourcen mit 3 Charts
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1074,18 +1074,12 @@
     <t>Personalkosten</t>
   </si>
   <si>
-    <t>Ergebnis-Prognose</t>
-  </si>
-  <si>
     <t>Risk fee</t>
   </si>
   <si>
     <t>Personnel Costs</t>
   </si>
   <si>
-    <t>Result Forecast</t>
-  </si>
-  <si>
     <t xml:space="preserve"> absolut </t>
   </si>
   <si>
@@ -1585,6 +1579,12 @@
   </si>
   <si>
     <t xml:space="preserve">Budget / Ergebnis Übersicht </t>
+  </si>
+  <si>
+    <t>Gewinn/Verlust</t>
+  </si>
+  <si>
+    <t>Profit/Loss</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1921,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A151" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A40" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2024,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,7 +2040,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2048,7 +2048,7 @@
         <v>337</v>
       </c>
       <c r="B15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2168,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2192,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
         <v>343</v>
       </c>
       <c r="B36" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>349</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2336,7 +2336,7 @@
         <v>350</v>
       </c>
       <c r="B51" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,10 +2349,10 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>351</v>
+        <v>520</v>
       </c>
       <c r="B53" t="s">
-        <v>354</v>
+        <v>521</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2464,15 +2464,15 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B68" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2480,7 +2480,7 @@
         <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
         <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
         <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2568,7 +2568,7 @@
         <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2592,15 +2592,15 @@
         <v>70</v>
       </c>
       <c r="B83" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B84" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2608,15 +2608,15 @@
         <v>71</v>
       </c>
       <c r="B85" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B86" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>72</v>
       </c>
       <c r="B87" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
         <v>73</v>
       </c>
       <c r="B88" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
         <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>75</v>
       </c>
       <c r="B90" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2664,7 +2664,7 @@
         <v>77</v>
       </c>
       <c r="B92" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
         <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
         <v>81</v>
       </c>
       <c r="B96" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,7 +2712,7 @@
         <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
         <v>86</v>
       </c>
       <c r="B101" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,7 +2744,7 @@
         <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
         <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
         <v>89</v>
       </c>
       <c r="B104" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
         <v>91</v>
       </c>
       <c r="B106" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,7 +2784,7 @@
         <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
         <v>93</v>
       </c>
       <c r="B108" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2800,7 +2800,7 @@
         <v>94</v>
       </c>
       <c r="B109" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
         <v>96</v>
       </c>
       <c r="B111" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <v>97</v>
       </c>
       <c r="B112" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2832,7 +2832,7 @@
         <v>98</v>
       </c>
       <c r="B113" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
         <v>99</v>
       </c>
       <c r="B114" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
         <v>100</v>
       </c>
       <c r="B115" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,10 +2869,10 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B118" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2880,7 +2880,7 @@
         <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>105</v>
       </c>
       <c r="B121" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2904,7 +2904,7 @@
         <v>106</v>
       </c>
       <c r="B122" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>109</v>
       </c>
       <c r="B125" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>110</v>
       </c>
       <c r="B126" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,7 +2952,7 @@
         <v>111</v>
       </c>
       <c r="B128" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2960,7 +2960,7 @@
         <v>112</v>
       </c>
       <c r="B129" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>113</v>
       </c>
       <c r="B130" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>114</v>
       </c>
       <c r="B131" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +2984,7 @@
         <v>115</v>
       </c>
       <c r="B132" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,7 +2992,7 @@
         <v>116</v>
       </c>
       <c r="B133" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>117</v>
       </c>
       <c r="B134" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>118</v>
       </c>
       <c r="B135" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>119</v>
       </c>
       <c r="B136" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>120</v>
       </c>
       <c r="B137" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>121</v>
       </c>
       <c r="B138" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>106</v>
       </c>
       <c r="B139" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>122</v>
       </c>
       <c r="B140" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>123</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>126</v>
       </c>
       <c r="B144" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>127</v>
       </c>
       <c r="B145" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>128</v>
       </c>
       <c r="B146" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3104,7 @@
         <v>129</v>
       </c>
       <c r="B147" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>130</v>
       </c>
       <c r="B148" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>133</v>
       </c>
       <c r="B151" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>123</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3152,7 @@
         <v>134</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3160,7 @@
         <v>135</v>
       </c>
       <c r="B154" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>136</v>
       </c>
       <c r="B155" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
         <v>139</v>
       </c>
       <c r="B158" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>140</v>
       </c>
       <c r="B159" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>141</v>
       </c>
       <c r="B160" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>143</v>
       </c>
       <c r="B162" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>144</v>
       </c>
       <c r="B163" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,7 +3240,7 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3256,7 +3256,7 @@
         <v>146</v>
       </c>
       <c r="B166" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3272,7 +3272,7 @@
         <v>148</v>
       </c>
       <c r="B168" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
         <v>149</v>
       </c>
       <c r="B169" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>150</v>
       </c>
       <c r="B170" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3296,7 @@
         <v>151</v>
       </c>
       <c r="B171" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
         <v>152</v>
       </c>
       <c r="B172" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,12 +3320,12 @@
         <v>153</v>
       </c>
       <c r="B174" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B175" t="s">
         <v>200</v>
@@ -3336,7 +3336,7 @@
         <v>154</v>
       </c>
       <c r="B176" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3344,7 +3344,7 @@
         <v>155</v>
       </c>
       <c r="B177" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>156</v>
       </c>
       <c r="B178" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3360,7 +3360,7 @@
         <v>157</v>
       </c>
       <c r="B179" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,7 +3368,7 @@
         <v>158</v>
       </c>
       <c r="B180" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
         <v>159</v>
       </c>
       <c r="B181" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>160</v>
       </c>
       <c r="B182" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>161</v>
       </c>
       <c r="B183" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3400,7 +3400,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3408,7 +3408,7 @@
         <v>162</v>
       </c>
       <c r="B185" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3416,7 +3416,7 @@
         <v>163</v>
       </c>
       <c r="B186" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
         <v>164</v>
       </c>
       <c r="B187" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3432,7 +3432,7 @@
         <v>165</v>
       </c>
       <c r="B188" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
         <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3448,7 +3448,7 @@
         <v>167</v>
       </c>
       <c r="B190" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,7 +3456,7 @@
         <v>168</v>
       </c>
       <c r="B191" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
         <v>169</v>
       </c>
       <c r="B192" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
         <v>171</v>
       </c>
       <c r="B194" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3488,7 +3488,7 @@
         <v>172</v>
       </c>
       <c r="B195" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,7 +3496,7 @@
         <v>173</v>
       </c>
       <c r="B196" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>174</v>
       </c>
       <c r="B197" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -3512,7 +3512,7 @@
         <v>175</v>
       </c>
       <c r="B198" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>177</v>
       </c>
       <c r="B200" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3536,7 +3536,7 @@
         <v>178</v>
       </c>
       <c r="B201" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3552,7 +3552,7 @@
         <v>180</v>
       </c>
       <c r="B203" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3560,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3613,10 +3613,10 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B211" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3661,10 +3661,10 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B217" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -3672,12 +3672,12 @@
         <v>242</v>
       </c>
       <c r="B218" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B219" t="s">
         <v>330</v>
@@ -3685,10 +3685,10 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B220" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B258" t="s">
         <v>329</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B259" t="s">
         <v>330</v>
@@ -4013,106 +4013,106 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B261" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B262" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B263" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B264" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B265" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B266" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B267" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B268" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B269" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B270" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B271" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>511</v>
+      </c>
+      <c r="B272" t="s">
         <v>513</v>
-      </c>
-      <c r="B272" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B273" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Windows pf Charts inkl Wechsel zw MPT und Mass-Edit Begonnen mit Projekte anlegen mit Ziel-Rendite
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="521">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -1008,12 +1008,6 @@
     <t>Overview Capacity Utilization</t>
   </si>
   <si>
-    <t>Details Capacity Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details Free Capacity </t>
-  </si>
-  <si>
     <t>Current &amp; Forecast Target Achievements</t>
   </si>
   <si>
@@ -1038,12 +1032,6 @@
     <t>Datenbank-Verbindung ist unterbrochen! &amp; vblf &amp; Projekthistorie konnte nicht geladen werden</t>
   </si>
   <si>
-    <t>Interne Kapazität</t>
-  </si>
-  <si>
-    <t>Internal Capacity</t>
-  </si>
-  <si>
     <t xml:space="preserve"> zu diesem Projekt gibt es noch keine Trend-Analyse, &amp; vblf &amp; da es noch nicht begonnen hat</t>
   </si>
   <si>
@@ -1122,21 +1110,12 @@
     <t xml:space="preserve">Overview Capacity Utilization </t>
   </si>
   <si>
-    <t xml:space="preserve">Details Capacity Overload </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details Überauslastung </t>
-  </si>
-  <si>
     <t>Projektliste</t>
   </si>
   <si>
     <t>Project List</t>
   </si>
   <si>
-    <t xml:space="preserve">Details freie Kapazität </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Personnel Costs </t>
   </si>
   <si>
@@ -1585,6 +1564,24 @@
   </si>
   <si>
     <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 3 freie Kapazität </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 3 Free Capacity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 3 Ressourcen Engpässe </t>
+  </si>
+  <si>
+    <t>Top 3 Resource Bottlenecks</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
+  </si>
+  <si>
+    <t>Capacity</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1921,8 +1918,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A40" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A239" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A263" sqref="A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
         <v>184</v>
@@ -1965,7 +1962,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s">
         <v>185</v>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>186</v>
@@ -2024,7 +2021,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,15 +2037,15 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2077,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2085,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,7 +2098,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B22" t="s">
         <v>210</v>
@@ -2120,7 +2117,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2125,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2133,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2141,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2149,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2157,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2165,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2173,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2181,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2189,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2197,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,10 +2210,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B36" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2221,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,7 +2229,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2240,7 +2237,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2248,7 +2245,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2253,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,7 +2261,7 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2269,7 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,12 +2277,12 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B45" t="s">
         <v>211</v>
@@ -2325,18 +2322,18 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B51" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,10 +2346,10 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="B53" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2453,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2464,15 +2461,15 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="B68" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2480,7 +2477,7 @@
         <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2488,7 +2485,7 @@
         <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,7 +2549,7 @@
         <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2560,7 +2557,7 @@
         <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2568,12 +2565,12 @@
         <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B81" t="s">
         <v>194</v>
@@ -2592,15 +2589,15 @@
         <v>70</v>
       </c>
       <c r="B83" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B84" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2608,15 +2605,15 @@
         <v>71</v>
       </c>
       <c r="B85" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B86" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,7 +2621,7 @@
         <v>72</v>
       </c>
       <c r="B87" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +2629,7 @@
         <v>73</v>
       </c>
       <c r="B88" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2637,7 @@
         <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2645,7 @@
         <v>75</v>
       </c>
       <c r="B90" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2656,7 +2653,7 @@
         <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2664,7 +2661,7 @@
         <v>77</v>
       </c>
       <c r="B92" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2672,7 +2669,7 @@
         <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2680,7 +2677,7 @@
         <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2688,7 +2685,7 @@
         <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,7 +2693,7 @@
         <v>81</v>
       </c>
       <c r="B96" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,7 +2709,7 @@
         <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2720,7 +2717,7 @@
         <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2728,7 +2725,7 @@
         <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2736,7 +2733,7 @@
         <v>86</v>
       </c>
       <c r="B101" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2744,7 +2741,7 @@
         <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2752,7 +2749,7 @@
         <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2760,7 +2757,7 @@
         <v>89</v>
       </c>
       <c r="B104" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2768,7 +2765,7 @@
         <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2776,7 +2773,7 @@
         <v>91</v>
       </c>
       <c r="B106" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2784,7 +2781,7 @@
         <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2792,7 +2789,7 @@
         <v>93</v>
       </c>
       <c r="B108" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2800,7 +2797,7 @@
         <v>94</v>
       </c>
       <c r="B109" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2816,7 +2813,7 @@
         <v>96</v>
       </c>
       <c r="B111" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2824,7 +2821,7 @@
         <v>97</v>
       </c>
       <c r="B112" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2832,7 +2829,7 @@
         <v>98</v>
       </c>
       <c r="B113" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2840,7 +2837,7 @@
         <v>99</v>
       </c>
       <c r="B114" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2848,7 +2845,7 @@
         <v>100</v>
       </c>
       <c r="B115" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,10 +2866,10 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B118" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2880,7 +2877,7 @@
         <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2896,7 +2893,7 @@
         <v>105</v>
       </c>
       <c r="B121" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2904,7 +2901,7 @@
         <v>106</v>
       </c>
       <c r="B122" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2928,7 +2925,7 @@
         <v>109</v>
       </c>
       <c r="B125" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2936,7 +2933,7 @@
         <v>110</v>
       </c>
       <c r="B126" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,7 +2941,7 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2952,7 +2949,7 @@
         <v>111</v>
       </c>
       <c r="B128" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2960,7 +2957,7 @@
         <v>112</v>
       </c>
       <c r="B129" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2968,7 +2965,7 @@
         <v>113</v>
       </c>
       <c r="B130" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +2973,7 @@
         <v>114</v>
       </c>
       <c r="B131" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +2981,7 @@
         <v>115</v>
       </c>
       <c r="B132" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,7 +2989,7 @@
         <v>116</v>
       </c>
       <c r="B133" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +2997,7 @@
         <v>117</v>
       </c>
       <c r="B134" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3005,7 @@
         <v>118</v>
       </c>
       <c r="B135" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3013,7 @@
         <v>119</v>
       </c>
       <c r="B136" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3021,7 @@
         <v>120</v>
       </c>
       <c r="B137" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3029,7 @@
         <v>121</v>
       </c>
       <c r="B138" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3037,7 @@
         <v>106</v>
       </c>
       <c r="B139" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3045,7 @@
         <v>122</v>
       </c>
       <c r="B140" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3053,7 @@
         <v>123</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3069,7 @@
         <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3077,7 @@
         <v>126</v>
       </c>
       <c r="B144" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3085,7 @@
         <v>127</v>
       </c>
       <c r="B145" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3093,7 @@
         <v>128</v>
       </c>
       <c r="B146" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3101,7 @@
         <v>129</v>
       </c>
       <c r="B147" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3109,7 @@
         <v>130</v>
       </c>
       <c r="B148" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3133,7 @@
         <v>133</v>
       </c>
       <c r="B151" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3141,7 @@
         <v>123</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3149,7 @@
         <v>134</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3157,7 @@
         <v>135</v>
       </c>
       <c r="B154" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3165,7 @@
         <v>136</v>
       </c>
       <c r="B155" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3173,7 @@
         <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3181,7 @@
         <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3192,7 +3189,7 @@
         <v>139</v>
       </c>
       <c r="B158" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3200,7 +3197,7 @@
         <v>140</v>
       </c>
       <c r="B159" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,7 +3205,7 @@
         <v>141</v>
       </c>
       <c r="B160" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3224,7 +3221,7 @@
         <v>143</v>
       </c>
       <c r="B162" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3232,7 +3229,7 @@
         <v>144</v>
       </c>
       <c r="B163" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3240,7 +3237,7 @@
         <v>44</v>
       </c>
       <c r="B164" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3256,7 +3253,7 @@
         <v>146</v>
       </c>
       <c r="B166" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3272,7 +3269,7 @@
         <v>148</v>
       </c>
       <c r="B168" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3280,7 +3277,7 @@
         <v>149</v>
       </c>
       <c r="B169" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3285,7 @@
         <v>150</v>
       </c>
       <c r="B170" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3293,7 @@
         <v>151</v>
       </c>
       <c r="B171" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3301,7 @@
         <v>152</v>
       </c>
       <c r="B172" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,12 +3317,12 @@
         <v>153</v>
       </c>
       <c r="B174" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B175" t="s">
         <v>200</v>
@@ -3336,7 +3333,7 @@
         <v>154</v>
       </c>
       <c r="B176" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3344,7 +3341,7 @@
         <v>155</v>
       </c>
       <c r="B177" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3352,7 +3349,7 @@
         <v>156</v>
       </c>
       <c r="B178" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3360,7 +3357,7 @@
         <v>157</v>
       </c>
       <c r="B179" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,7 +3365,7 @@
         <v>158</v>
       </c>
       <c r="B180" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3376,7 +3373,7 @@
         <v>159</v>
       </c>
       <c r="B181" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3384,7 +3381,7 @@
         <v>160</v>
       </c>
       <c r="B182" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3392,7 +3389,7 @@
         <v>161</v>
       </c>
       <c r="B183" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3400,7 +3397,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3408,7 +3405,7 @@
         <v>162</v>
       </c>
       <c r="B185" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3416,7 +3413,7 @@
         <v>163</v>
       </c>
       <c r="B186" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3424,7 +3421,7 @@
         <v>164</v>
       </c>
       <c r="B187" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3432,7 +3429,7 @@
         <v>165</v>
       </c>
       <c r="B188" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3440,7 +3437,7 @@
         <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3448,7 +3445,7 @@
         <v>167</v>
       </c>
       <c r="B190" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,7 +3453,7 @@
         <v>168</v>
       </c>
       <c r="B191" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3464,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="B192" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3480,7 +3477,7 @@
         <v>171</v>
       </c>
       <c r="B194" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3488,7 +3485,7 @@
         <v>172</v>
       </c>
       <c r="B195" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3496,7 +3493,7 @@
         <v>173</v>
       </c>
       <c r="B196" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3504,7 +3501,7 @@
         <v>174</v>
       </c>
       <c r="B197" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -3512,7 +3509,7 @@
         <v>175</v>
       </c>
       <c r="B198" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3528,7 +3525,7 @@
         <v>177</v>
       </c>
       <c r="B200" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3536,7 +3533,7 @@
         <v>178</v>
       </c>
       <c r="B201" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3552,7 +3549,7 @@
         <v>180</v>
       </c>
       <c r="B203" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3560,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3613,10 +3610,10 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="B211" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3661,10 +3658,10 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B217" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -3672,23 +3669,23 @@
         <v>242</v>
       </c>
       <c r="B218" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>371</v>
+        <v>515</v>
       </c>
       <c r="B219" t="s">
-        <v>330</v>
+        <v>516</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>368</v>
+        <v>517</v>
       </c>
       <c r="B220" t="s">
-        <v>367</v>
+        <v>518</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -3736,7 +3733,7 @@
         <v>248</v>
       </c>
       <c r="B226" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3848,7 +3845,7 @@
         <v>262</v>
       </c>
       <c r="B240" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3976,7 +3973,7 @@
         <v>322</v>
       </c>
       <c r="B256" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -3989,130 +3986,130 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>368</v>
+        <v>517</v>
       </c>
       <c r="B258" t="s">
-        <v>329</v>
+        <v>518</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>371</v>
+        <v>515</v>
       </c>
       <c r="B259" t="s">
-        <v>330</v>
+        <v>516</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>339</v>
+        <v>519</v>
       </c>
       <c r="B260" t="s">
-        <v>340</v>
+        <v>520</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B261" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B262" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>489</v>
+      </c>
+      <c r="B263" t="s">
         <v>496</v>
-      </c>
-      <c r="B263" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
+        <v>490</v>
+      </c>
+      <c r="B264" t="s">
         <v>497</v>
-      </c>
-      <c r="B264" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B265" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B266" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B267" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B268" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B269" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="B270" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B271" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B272" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="B273" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report alles auf Englisch, auch wenn sowohl interaktiv als auch Report-Texte benutzt werden. Damit kann interaktive Sprache englisch sein und Report Sprache irgendeine vorhandene andere.
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\Documents\Visual Studio 2013\Projects\ProjectBoard\Projectboard\ClassLibrary1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="13020"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="529">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -1582,6 +1587,30 @@
   </si>
   <si>
     <t>Capacity</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>Summe über alle Projekte</t>
+  </si>
+  <si>
+    <t>Sum over all projects</t>
+  </si>
+  <si>
+    <t>Platzhalter</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>zugeordnet</t>
+  </si>
+  <si>
+    <t>assigned</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +1936,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1916,10 +1945,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B273"/>
+  <dimension ref="A1:B277"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A239" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A263" sqref="A263"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A257" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B274" sqref="B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4112,6 +4141,38 @@
         <v>501</v>
       </c>
     </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>521</v>
+      </c>
+      <c r="B274" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>523</v>
+      </c>
+      <c r="B275" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>525</v>
+      </c>
+      <c r="B276" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>527</v>
+      </c>
+      <c r="B277" t="s">
+        <v>528</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Report Texte sollten neu übersetzt werden .. in der Projektliste ein paar Korrekturen gemacht: Default ist jetzt das Ausweisen von T€ (nicht mehr PT)
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1458,12 +1458,6 @@
     <t>Budget &amp; vblf &amp; (T€)</t>
   </si>
   <si>
-    <t>P.-Bedarfe &amp; vblf &amp; (PT)</t>
-  </si>
-  <si>
-    <t>E.-Kosten &amp; vblf &amp; (T€)</t>
-  </si>
-  <si>
     <t>Stand vom</t>
   </si>
   <si>
@@ -1473,9 +1467,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Ext.-Cost &amp; vblf &amp; (T€)</t>
-  </si>
-  <si>
     <t>Ergebnis &amp; vblf &amp; (T€)</t>
   </si>
   <si>
@@ -1509,9 +1500,6 @@
     <t xml:space="preserve"> (PD)</t>
   </si>
   <si>
-    <t>P.-Needs &amp; vblf &amp; (PD)</t>
-  </si>
-  <si>
     <t>Overview Budget / Result</t>
   </si>
   <si>
@@ -1603,6 +1591,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Personnel Costs</t>
+  </si>
+  <si>
+    <t>S.-Kosten &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Oth.-Cost &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>P.-Kosten &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>P.-Cost &amp; vblf &amp; (T€)</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1928,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1939,8 +1939,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B277"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A190" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A259" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B53" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B68" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
         <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3439,50 +3439,50 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B187" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B188" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B189" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B190" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B191" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B192" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3631,10 +3631,10 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B211" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3690,23 +3690,23 @@
         <v>235</v>
       </c>
       <c r="B218" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B219" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B220" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -4007,26 +4007,26 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B258" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B259" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B260" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
         <v>475</v>
       </c>
       <c r="B263" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
         <v>476</v>
       </c>
       <c r="B264" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -4079,90 +4079,90 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>479</v>
+        <v>526</v>
       </c>
       <c r="B267" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>480</v>
+        <v>524</v>
       </c>
       <c r="B268" t="s">
-        <v>484</v>
+        <v>525</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B269" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B270" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>485</v>
+      </c>
+      <c r="B271" t="s">
         <v>488</v>
-      </c>
-      <c r="B271" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B272" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B273" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B274" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B275" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B276" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B277" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge capexAllianz into Master
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1458,12 +1458,6 @@
     <t>Budget &amp; vblf &amp; (T€)</t>
   </si>
   <si>
-    <t>P.-Bedarfe &amp; vblf &amp; (PT)</t>
-  </si>
-  <si>
-    <t>E.-Kosten &amp; vblf &amp; (T€)</t>
-  </si>
-  <si>
     <t>Stand vom</t>
   </si>
   <si>
@@ -1473,9 +1467,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Ext.-Cost &amp; vblf &amp; (T€)</t>
-  </si>
-  <si>
     <t>Ergebnis &amp; vblf &amp; (T€)</t>
   </si>
   <si>
@@ -1509,9 +1500,6 @@
     <t xml:space="preserve"> (PD)</t>
   </si>
   <si>
-    <t>P.-Needs &amp; vblf &amp; (PD)</t>
-  </si>
-  <si>
     <t>Overview Budget / Result</t>
   </si>
   <si>
@@ -1603,6 +1591,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Personnel Costs</t>
+  </si>
+  <si>
+    <t>S.-Kosten &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Oth.-Cost &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>P.-Kosten &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>P.-Cost &amp; vblf &amp; (T€)</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1928,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1939,8 +1939,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B277"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A190" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A259" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B53" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B68" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
         <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3439,50 +3439,50 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B187" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B188" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B189" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B190" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B191" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B192" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3631,10 +3631,10 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B211" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3690,23 +3690,23 @@
         <v>235</v>
       </c>
       <c r="B218" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B219" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B220" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -4007,26 +4007,26 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B258" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B259" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B260" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
         <v>475</v>
       </c>
       <c r="B263" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
         <v>476</v>
       </c>
       <c r="B264" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -4079,90 +4079,90 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>479</v>
+        <v>526</v>
       </c>
       <c r="B267" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>480</v>
+        <v>524</v>
       </c>
       <c r="B268" t="s">
-        <v>484</v>
+        <v>525</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B269" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B270" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>485</v>
+      </c>
+      <c r="B271" t="s">
         <v>488</v>
-      </c>
-      <c r="B271" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B272" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B273" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B274" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B275" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B276" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B277" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projectboard: ReportTexte.xlsx appended with strings for smartInfo Create; repMessages now from VCSetting
</commit_message>
<xml_diff>
--- a/Projectboard/ClassLibrary1/ReportTexte.xlsx
+++ b/Projectboard/ClassLibrary1/ReportTexte.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UteRittinghaus-Koyte\Dokumente\VISBO-NativeClients\visbo-projectboard\Projectboard\ClassLibrary1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86263183-B538-46AD-89C5-FA813C32136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="13020"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="555">
   <si>
     <t xml:space="preserve"> Soll-Ist Kostenart </t>
   </si>
@@ -1603,12 +1609,93 @@
   </si>
   <si>
     <t>P.-Cost &amp; vblf &amp; (T€)</t>
+  </si>
+  <si>
+    <t>Ist-Werte</t>
+  </si>
+  <si>
+    <t>Actual-to-date</t>
+  </si>
+  <si>
+    <t>Ist-Werte (Summe Portfolio)</t>
+  </si>
+  <si>
+    <t>Actual-to-date (Sum OF Portfolio)</t>
+  </si>
+  <si>
+    <t>Forecast (ETC)</t>
+  </si>
+  <si>
+    <t>Actual and Forecast (EAC)</t>
+  </si>
+  <si>
+    <t>Last ETC</t>
+  </si>
+  <si>
+    <t>Letzter ETC</t>
+  </si>
+  <si>
+    <t>Monthly Needs (Sum of Portfolio)</t>
+  </si>
+  <si>
+    <t>monatl. Bedarfe (alle Projekte des Portfolios)</t>
+  </si>
+  <si>
+    <t>Baseline (BAC)</t>
+  </si>
+  <si>
+    <t>Order-Value</t>
+  </si>
+  <si>
+    <t>Auftragswert</t>
+  </si>
+  <si>
+    <t>Invoices (Baseline)</t>
+  </si>
+  <si>
+    <t>Rechnungen (Baseline)</t>
+  </si>
+  <si>
+    <t>Gesamt Kapazität</t>
+  </si>
+  <si>
+    <t>Total Capacity</t>
+  </si>
+  <si>
+    <t>interne Kapazität</t>
+  </si>
+  <si>
+    <t>intern Capacity</t>
+  </si>
+  <si>
+    <t>Summe Portfolio</t>
+  </si>
+  <si>
+    <t>Sum of Portfolio</t>
+  </si>
+  <si>
+    <t>Summe interner Mitarbeiter</t>
+  </si>
+  <si>
+    <t>Sum of all intern employees</t>
+  </si>
+  <si>
+    <t>Summe pro Monat</t>
+  </si>
+  <si>
+    <t>Monthly Sum</t>
+  </si>
+  <si>
+    <t>Rechnungen (akt. Plan)</t>
+  </si>
+  <si>
+    <t>Invoices (cur. Plan)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1650,12 +1737,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1928,19 +2013,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B277"/>
+  <dimension ref="A1:B292"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A259" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A271" sqref="A271"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A265" colorId="22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B296" sqref="B296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,7 +2059,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1993,7 +2078,7 @@
       <c r="A6" t="s">
         <v>327</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2033,7 +2118,7 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2049,7 +2134,7 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2073,7 +2158,7 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2345,7 +2430,7 @@
       <c r="A50" t="s">
         <v>338</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>340</v>
       </c>
     </row>
@@ -2401,7 +2486,7 @@
       <c r="A57" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2513,7 +2598,7 @@
       <c r="A71" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3073,7 +3158,7 @@
       <c r="A141" t="s">
         <v>123</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="1" t="s">
         <v>448</v>
       </c>
     </row>
@@ -3081,7 +3166,7 @@
       <c r="A142" t="s">
         <v>124</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3161,7 +3246,7 @@
       <c r="A152" t="s">
         <v>123</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="1" t="s">
         <v>368</v>
       </c>
     </row>
@@ -3169,7 +3254,7 @@
       <c r="A153" t="s">
         <v>134</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" s="1" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4163,6 +4248,126 @@
       </c>
       <c r="B277" t="s">
         <v>510</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>528</v>
+      </c>
+      <c r="B278" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>530</v>
+      </c>
+      <c r="B279" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>532</v>
+      </c>
+      <c r="B280" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>533</v>
+      </c>
+      <c r="B281" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>535</v>
+      </c>
+      <c r="B282" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>537</v>
+      </c>
+      <c r="B283" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>538</v>
+      </c>
+      <c r="B284" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>540</v>
+      </c>
+      <c r="B285" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>542</v>
+      </c>
+      <c r="B286" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>553</v>
+      </c>
+      <c r="B287" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>543</v>
+      </c>
+      <c r="B288" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>545</v>
+      </c>
+      <c r="B289" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>547</v>
+      </c>
+      <c r="B290" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>549</v>
+      </c>
+      <c r="B291" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>551</v>
+      </c>
+      <c r="B292" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>